<commit_message>
lyrics txt files generated 90%
</commit_message>
<xml_diff>
--- a/exports/Top 100.xlsx
+++ b/exports/Top 100.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="336">
   <si>
     <t>artist</t>
   </si>
@@ -88,27 +88,27 @@
     <t>Frank Ocean</t>
   </si>
   <si>
+    <t>Dream Theater</t>
+  </si>
+  <si>
     <t>Car Seat Headrest</t>
   </si>
   <si>
     <t>Brand New</t>
   </si>
   <si>
-    <t>Dream Theater</t>
+    <t>Kendrick Lamar</t>
+  </si>
+  <si>
+    <t>Bon Iver</t>
   </si>
   <si>
     <t>Deafheaven</t>
   </si>
   <si>
-    <t>Kendrick Lamar</t>
-  </si>
-  <si>
     <t>Fleet Foxes</t>
   </si>
   <si>
-    <t>Bon Iver</t>
-  </si>
-  <si>
     <t>My Chemical Romance</t>
   </si>
   <si>
@@ -166,48 +166,48 @@
     <t>Interpol</t>
   </si>
   <si>
+    <t>Pulp</t>
+  </si>
+  <si>
     <t>Iron Maiden</t>
   </si>
   <si>
     <t>Fleetwood Mac</t>
   </si>
   <si>
-    <t>Pulp</t>
+    <t>Beach House</t>
+  </si>
+  <si>
+    <t>Have A Nice Life</t>
+  </si>
+  <si>
+    <t>Death Cab For Cutie</t>
+  </si>
+  <si>
+    <t>The Strokes</t>
+  </si>
+  <si>
+    <t>Deftones</t>
+  </si>
+  <si>
+    <t>The Cure</t>
+  </si>
+  <si>
+    <t>Metallica</t>
+  </si>
+  <si>
+    <t>Travis Scott</t>
+  </si>
+  <si>
+    <t>MØL</t>
+  </si>
+  <si>
+    <t>twenty one pilots</t>
   </si>
   <si>
     <t>Charli XCX</t>
   </si>
   <si>
-    <t>Beach House</t>
-  </si>
-  <si>
-    <t>Have A Nice Life</t>
-  </si>
-  <si>
-    <t>Death Cab For Cutie</t>
-  </si>
-  <si>
-    <t>The Strokes</t>
-  </si>
-  <si>
-    <t>Deftones</t>
-  </si>
-  <si>
-    <t>The Cure</t>
-  </si>
-  <si>
-    <t>Metallica</t>
-  </si>
-  <si>
-    <t>Travis Scott</t>
-  </si>
-  <si>
-    <t>MØL</t>
-  </si>
-  <si>
-    <t>KIDS SEE GHOSTS</t>
-  </si>
-  <si>
     <t>Bonobo</t>
   </si>
   <si>
@@ -259,27 +259,27 @@
     <t>blonde</t>
   </si>
   <si>
+    <t>metropolis part 2: scenes from a memory</t>
+  </si>
+  <si>
     <t>teens of denial</t>
   </si>
   <si>
     <t>the devil and god are raging inside me</t>
   </si>
   <si>
-    <t>metropolis part 2: scenes from a memory</t>
+    <t>good kid, m.a.a.d city</t>
+  </si>
+  <si>
+    <t>for emma, forever ago</t>
   </si>
   <si>
     <t>sunbather</t>
   </si>
   <si>
-    <t>good kid, m.a.a.d city</t>
-  </si>
-  <si>
     <t>helplessness blues</t>
   </si>
   <si>
-    <t>for emma, forever ago</t>
-  </si>
-  <si>
     <t>the black parade</t>
   </si>
   <si>
@@ -361,48 +361,48 @@
     <t>turn on the bright lights</t>
   </si>
   <si>
+    <t>different class</t>
+  </si>
+  <si>
     <t>powerslave</t>
   </si>
   <si>
     <t>rumours</t>
   </si>
   <si>
-    <t>different class</t>
+    <t>bloom</t>
+  </si>
+  <si>
+    <t>deathconsciousness</t>
+  </si>
+  <si>
+    <t>transatlanticism</t>
+  </si>
+  <si>
+    <t>is this it</t>
+  </si>
+  <si>
+    <t>white pony</t>
+  </si>
+  <si>
+    <t>disintegration</t>
+  </si>
+  <si>
+    <t>master of puppets</t>
+  </si>
+  <si>
+    <t>astroworld</t>
+  </si>
+  <si>
+    <t>jord</t>
+  </si>
+  <si>
+    <t>trench</t>
   </si>
   <si>
     <t>pop 2</t>
   </si>
   <si>
-    <t>bloom</t>
-  </si>
-  <si>
-    <t>deathconsciousness</t>
-  </si>
-  <si>
-    <t>transatlanticism</t>
-  </si>
-  <si>
-    <t>is this it</t>
-  </si>
-  <si>
-    <t>white pony</t>
-  </si>
-  <si>
-    <t>disintegration</t>
-  </si>
-  <si>
-    <t>master of puppets</t>
-  </si>
-  <si>
-    <t>astroworld</t>
-  </si>
-  <si>
-    <t>jord</t>
-  </si>
-  <si>
-    <t>kids see ghosts</t>
-  </si>
-  <si>
     <t>damn</t>
   </si>
   <si>
@@ -454,9 +454,6 @@
     <t>the suburbs</t>
   </si>
   <si>
-    <t>graduation</t>
-  </si>
-  <si>
     <t>the moon &amp; antarctica</t>
   </si>
   <si>
@@ -487,24 +484,24 @@
     <t>Alternative R&amp;B</t>
   </si>
   <si>
+    <t>Progressive Metal</t>
+  </si>
+  <si>
     <t>Lo-Fi Indie Rock</t>
   </si>
   <si>
     <t>Emo</t>
   </si>
   <si>
-    <t>Progressive Metal</t>
+    <t>Conscious Hip Hop</t>
+  </si>
+  <si>
+    <t>Indie Folk</t>
   </si>
   <si>
     <t>Blackgaze</t>
   </si>
   <si>
-    <t>Conscious Hip Hop</t>
-  </si>
-  <si>
-    <t>Indie Folk</t>
-  </si>
-  <si>
     <t>Pop Punk</t>
   </si>
   <si>
@@ -547,27 +544,30 @@
     <t>Disco Punk</t>
   </si>
   <si>
+    <t>Britpop</t>
+  </si>
+  <si>
     <t>Heavy Metal</t>
   </si>
   <si>
-    <t>Britpop</t>
+    <t>Dream Pop</t>
+  </si>
+  <si>
+    <t>Alternative Metal</t>
+  </si>
+  <si>
+    <t>Goth Rock</t>
+  </si>
+  <si>
+    <t>Psychedelic Trap</t>
+  </si>
+  <si>
+    <t>Indie Pop</t>
   </si>
   <si>
     <t>Electropop</t>
   </si>
   <si>
-    <t>Dream Pop</t>
-  </si>
-  <si>
-    <t>Alternative Metal</t>
-  </si>
-  <si>
-    <t>Goth Rock</t>
-  </si>
-  <si>
-    <t>Psychedelic Trap</t>
-  </si>
-  <si>
     <t>Ambient Electronic</t>
   </si>
   <si>
@@ -580,9 +580,6 @@
     <t>Trip-Hop</t>
   </si>
   <si>
-    <t>Indie Pop</t>
-  </si>
-  <si>
     <t>2010</t>
   </si>
   <si>
@@ -598,24 +595,24 @@
     <t>2016</t>
   </si>
   <si>
+    <t>1999</t>
+  </si>
+  <si>
     <t>2006</t>
   </si>
   <si>
-    <t>1999</t>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2008</t>
   </si>
   <si>
     <t>2013</t>
   </si>
   <si>
-    <t>2012</t>
-  </si>
-  <si>
     <t>2011</t>
   </si>
   <si>
-    <t>2008</t>
-  </si>
-  <si>
     <t>2001</t>
   </si>
   <si>
@@ -685,15 +682,15 @@
     <t>12</t>
   </si>
   <si>
+    <t>11.5</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>10.5</t>
   </si>
   <si>
-    <t>11.5</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>7.5</t>
   </si>
   <si>
@@ -703,7 +700,7 @@
     <t>31.5</t>
   </si>
   <si>
-    <t>31</t>
+    <t>30.5</t>
   </si>
   <si>
     <t>30</t>
@@ -748,27 +745,27 @@
     <t>Self Control</t>
   </si>
   <si>
+    <t>Home</t>
+  </si>
+  <si>
     <t>Drugs With Friends</t>
   </si>
   <si>
     <t>Jesus Christ</t>
   </si>
   <si>
-    <t>Home</t>
+    <t>m.a.a.d city</t>
+  </si>
+  <si>
+    <t>Re: Stacks</t>
   </si>
   <si>
     <t>Dream House</t>
   </si>
   <si>
-    <t>m.a.a.d city</t>
-  </si>
-  <si>
     <t>Helplessness Blues</t>
   </si>
   <si>
-    <t>Re: Stacks</t>
-  </si>
-  <si>
     <t>Welcome To The Black Parade</t>
   </si>
   <si>
@@ -850,48 +847,48 @@
     <t>PDA</t>
   </si>
   <si>
+    <t>Common People</t>
+  </si>
+  <si>
     <t>Rime of the Ancient Mariner</t>
   </si>
   <si>
     <t>Dreams</t>
   </si>
   <si>
-    <t>Common People</t>
+    <t>Lazuli</t>
+  </si>
+  <si>
+    <t>Bloodhail</t>
+  </si>
+  <si>
+    <t>Tiny Vessels</t>
+  </si>
+  <si>
+    <t>Hard To Explain</t>
+  </si>
+  <si>
+    <t>Change (In The House Of Flies)</t>
+  </si>
+  <si>
+    <t>Fascination Street</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>STOP TRYING TO BE GOD</t>
+  </si>
+  <si>
+    <t>Penumbra</t>
+  </si>
+  <si>
+    <t>Neon Gravestones</t>
   </si>
   <si>
     <t>Track 10</t>
   </si>
   <si>
-    <t>Lazuli</t>
-  </si>
-  <si>
-    <t>Bloodhail</t>
-  </si>
-  <si>
-    <t>Tiny Vessels</t>
-  </si>
-  <si>
-    <t>Hard To Explain</t>
-  </si>
-  <si>
-    <t>Change (In The House Of Flies)</t>
-  </si>
-  <si>
-    <t>Fascination Street</t>
-  </si>
-  <si>
-    <t>Battery</t>
-  </si>
-  <si>
-    <t>STOP TRYING TO BE GOD</t>
-  </si>
-  <si>
-    <t>Penumbra</t>
-  </si>
-  <si>
-    <t>4th Dimension</t>
-  </si>
-  <si>
     <t>HUMBLE</t>
   </si>
   <si>
@@ -943,9 +940,6 @@
     <t>Sprawl II</t>
   </si>
   <si>
-    <t>Flashing Lights</t>
-  </si>
-  <si>
     <t>3rd Planet</t>
   </si>
   <si>
@@ -970,13 +964,13 @@
     <t>9.36</t>
   </si>
   <si>
+    <t>9.27</t>
+  </si>
+  <si>
+    <t>9.35</t>
+  </si>
+  <si>
     <t>9.25</t>
-  </si>
-  <si>
-    <t>9.27</t>
-  </si>
-  <si>
-    <t>9.35</t>
   </si>
   <si>
     <t>9.13</t>
@@ -1385,7 +1379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T73"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1461,34 +1455,34 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M2">
         <v>68</v>
@@ -1523,34 +1517,34 @@
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M3">
         <v>55</v>
@@ -1585,43 +1579,43 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M4">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="N4">
         <v>0.2781818181818181</v>
       </c>
       <c r="O4">
-        <v>0.2745454545454545</v>
+        <v>0.2745454545454546</v>
       </c>
       <c r="P4">
         <v>0.05545454545454546</v>
@@ -1647,46 +1641,46 @@
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M5">
         <v>25</v>
       </c>
       <c r="N5">
-        <v>0.2073913043478261</v>
+        <v>0.207391304347826</v>
       </c>
       <c r="O5">
-        <v>0.3100000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="P5">
-        <v>0.04565217391304349</v>
+        <v>0.0456521739130435</v>
       </c>
       <c r="Q5">
         <v>0.2530434782608696</v>
@@ -1709,43 +1703,43 @@
         <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M6">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N6">
         <v>0.7185294117647061</v>
       </c>
       <c r="O6">
-        <v>0.5014705882352941</v>
+        <v>0.501470588235294</v>
       </c>
       <c r="P6">
         <v>0.1923529411764706</v>
@@ -1771,58 +1765,58 @@
         <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
         <v>193</v>
       </c>
       <c r="F7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="M7">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="N7">
-        <v>0.1725</v>
+        <v>0.2241666666666666</v>
       </c>
       <c r="O7">
-        <v>0.44</v>
+        <v>0.405</v>
       </c>
       <c r="P7">
-        <v>0.04916666666666667</v>
+        <v>0.1075</v>
       </c>
       <c r="Q7">
-        <v>0.3383333333333334</v>
+        <v>0.2945833333333334</v>
       </c>
       <c r="R7">
-        <v>0.5508333333333333</v>
+        <v>0.68125</v>
       </c>
       <c r="S7">
-        <v>0.1416666666666667</v>
+        <v>0.3000000000000001</v>
       </c>
       <c r="T7">
-        <v>0.05583333333333333</v>
+        <v>0.1470833333333333</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1833,58 +1827,58 @@
         <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H8" t="s">
         <v>218</v>
       </c>
       <c r="I8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="L8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M8">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="N8">
-        <v>0.1458333333333333</v>
+        <v>0.1725</v>
       </c>
       <c r="O8">
-        <v>0.425</v>
+        <v>0.44</v>
       </c>
       <c r="P8">
-        <v>0.04666666666666667</v>
+        <v>0.04916666666666667</v>
       </c>
       <c r="Q8">
-        <v>0.215</v>
+        <v>0.3383333333333334</v>
       </c>
       <c r="R8">
-        <v>0.6633333333333333</v>
+        <v>0.5508333333333334</v>
       </c>
       <c r="S8">
-        <v>0.17</v>
+        <v>0.1416666666666667</v>
       </c>
       <c r="T8">
-        <v>0.1008333333333333</v>
+        <v>0.05583333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1895,58 +1889,58 @@
         <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F9" t="s">
         <v>218</v>
       </c>
       <c r="G9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="N9">
-        <v>0.2241666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="O9">
-        <v>0.405</v>
+        <v>0.425</v>
       </c>
       <c r="P9">
-        <v>0.1075</v>
+        <v>0.04666666666666667</v>
       </c>
       <c r="Q9">
-        <v>0.2945833333333334</v>
+        <v>0.215</v>
       </c>
       <c r="R9">
-        <v>0.68125</v>
+        <v>0.6633333333333333</v>
       </c>
       <c r="S9">
-        <v>0.3000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="T9">
-        <v>0.1470833333333333</v>
+        <v>0.1008333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1957,58 +1951,58 @@
         <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F10" t="s">
         <v>217</v>
       </c>
       <c r="G10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H10" t="s">
         <v>218</v>
       </c>
       <c r="I10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N10">
-        <v>0.3342857142857142</v>
+        <v>0.1235714285714286</v>
       </c>
       <c r="O10">
-        <v>0.2371428571428571</v>
+        <v>0.5921428571428571</v>
       </c>
       <c r="P10">
-        <v>0.05571428571428572</v>
+        <v>0.2921428571428571</v>
       </c>
       <c r="Q10">
-        <v>0.09999999999999999</v>
+        <v>0.3114285714285714</v>
       </c>
       <c r="R10">
-        <v>0.6185714285714285</v>
+        <v>0.6657142857142857</v>
       </c>
       <c r="S10">
-        <v>0.1871428571428571</v>
+        <v>0.3307142857142857</v>
       </c>
       <c r="T10">
-        <v>0.89</v>
+        <v>0.0007142857142857143</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -2019,58 +2013,58 @@
         <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F11" t="s">
         <v>218</v>
       </c>
       <c r="G11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M11">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="N11">
-        <v>0.1235714285714286</v>
+        <v>0.7677777777777778</v>
       </c>
       <c r="O11">
-        <v>0.5921428571428571</v>
+        <v>0.5622222222222223</v>
       </c>
       <c r="P11">
-        <v>0.2921428571428571</v>
+        <v>0.05222222222222222</v>
       </c>
       <c r="Q11">
-        <v>0.3114285714285714</v>
+        <v>0.2977777777777778</v>
       </c>
       <c r="R11">
-        <v>0.6657142857142857</v>
+        <v>0.2933333333333333</v>
       </c>
       <c r="S11">
-        <v>0.3307142857142858</v>
+        <v>0.1488888888888889</v>
       </c>
       <c r="T11">
-        <v>0.0007142857142857143</v>
+        <v>0.2311111111111111</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -2084,55 +2078,55 @@
         <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G12" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K12" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="L12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M12">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="N12">
-        <v>0.4758333333333333</v>
+        <v>0.3342857142857142</v>
       </c>
       <c r="O12">
-        <v>0.41</v>
+        <v>0.2371428571428571</v>
       </c>
       <c r="P12">
-        <v>0.03333333333333335</v>
+        <v>0.05571428571428572</v>
       </c>
       <c r="Q12">
-        <v>0.3425</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="R12">
-        <v>0.4308333333333333</v>
+        <v>0.6185714285714285</v>
       </c>
       <c r="S12">
-        <v>0.1225</v>
+        <v>0.1871428571428571</v>
       </c>
       <c r="T12">
-        <v>0.0825</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -2143,58 +2137,58 @@
         <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K13" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="L13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M13">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="N13">
-        <v>0.7677777777777778</v>
+        <v>0.4758333333333333</v>
       </c>
       <c r="O13">
-        <v>0.5622222222222222</v>
+        <v>0.4099999999999999</v>
       </c>
       <c r="P13">
-        <v>0.05222222222222222</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="Q13">
-        <v>0.2977777777777778</v>
+        <v>0.3425</v>
       </c>
       <c r="R13">
-        <v>0.2933333333333333</v>
+        <v>0.4308333333333333</v>
       </c>
       <c r="S13">
-        <v>0.1488888888888889</v>
+        <v>0.1225</v>
       </c>
       <c r="T13">
-        <v>0.2311111111111111</v>
+        <v>0.0825</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -2205,34 +2199,34 @@
         <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E14" t="s">
         <v>194</v>
       </c>
       <c r="F14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M14">
         <v>22</v>
@@ -2250,10 +2244,10 @@
         <v>0.36</v>
       </c>
       <c r="R14">
-        <v>0.8014285714285716</v>
+        <v>0.8014285714285714</v>
       </c>
       <c r="S14">
-        <v>0.2064285714285714</v>
+        <v>0.2064285714285715</v>
       </c>
       <c r="T14">
         <v>0.001428571428571429</v>
@@ -2267,37 +2261,37 @@
         <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M15">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="N15">
         <v>0.601</v>
@@ -2312,7 +2306,7 @@
         <v>0.191</v>
       </c>
       <c r="R15">
-        <v>0.3924999999999999</v>
+        <v>0.3925</v>
       </c>
       <c r="S15">
         <v>0.1425</v>
@@ -2329,34 +2323,34 @@
         <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M16">
         <v>80</v>
@@ -2391,34 +2385,34 @@
         <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G17" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="L17" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M17">
         <v>26</v>
@@ -2427,13 +2421,13 @@
         <v>0.3846666666666667</v>
       </c>
       <c r="O17">
-        <v>0.5946666666666667</v>
+        <v>0.5946666666666666</v>
       </c>
       <c r="P17">
-        <v>0.1546666666666667</v>
+        <v>0.1546666666666666</v>
       </c>
       <c r="Q17">
-        <v>0.5473333333333332</v>
+        <v>0.5473333333333333</v>
       </c>
       <c r="R17">
         <v>0.6039999999999999</v>
@@ -2453,49 +2447,49 @@
         <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K18" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L18" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M18">
         <v>33</v>
       </c>
       <c r="N18">
-        <v>0.8736363636363634</v>
+        <v>0.8736363636363635</v>
       </c>
       <c r="O18">
-        <v>0.6145454545454545</v>
+        <v>0.6145454545454546</v>
       </c>
       <c r="P18">
         <v>0.04272727272727272</v>
       </c>
       <c r="Q18">
-        <v>0.5027272727272728</v>
+        <v>0.5027272727272727</v>
       </c>
       <c r="R18">
         <v>0.3190909090909091</v>
@@ -2515,34 +2509,34 @@
         <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K19" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="L19" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M19">
         <v>6</v>
@@ -2551,7 +2545,7 @@
         <v>0.2869230769230769</v>
       </c>
       <c r="O19">
-        <v>0.6869230769230771</v>
+        <v>0.6869230769230769</v>
       </c>
       <c r="P19">
         <v>0.04384615384615385</v>
@@ -2571,40 +2565,40 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E20" t="s">
         <v>198</v>
       </c>
       <c r="F20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K20" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M20">
         <v>80</v>
@@ -2633,49 +2627,49 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L21" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M21">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N21">
         <v>0.5454545454545454</v>
       </c>
       <c r="O21">
-        <v>0.5363636363636363</v>
+        <v>0.5363636363636364</v>
       </c>
       <c r="P21">
         <v>0.03090909090909092</v>
@@ -2701,37 +2695,37 @@
         <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K22" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L22" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M22">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N22">
         <v>0.02307692307692307</v>
@@ -2740,13 +2734,13 @@
         <v>0.4615384615384616</v>
       </c>
       <c r="P22">
-        <v>0.09538461538461539</v>
+        <v>0.0953846153846154</v>
       </c>
       <c r="Q22">
         <v>0.4392307692307693</v>
       </c>
       <c r="R22">
-        <v>0.8461538461538463</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="S22">
         <v>0.1876923076923077</v>
@@ -2763,34 +2757,34 @@
         <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L23" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M23">
         <v>14</v>
@@ -2825,34 +2819,34 @@
         <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L24" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M24">
         <v>113</v>
@@ -2867,7 +2861,7 @@
         <v>0.04600000000000001</v>
       </c>
       <c r="Q24">
-        <v>0.6133333333333333</v>
+        <v>0.6133333333333332</v>
       </c>
       <c r="R24">
         <v>0.6093333333333334</v>
@@ -2887,55 +2881,55 @@
         <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K25" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M25">
         <v>14</v>
       </c>
       <c r="N25">
-        <v>0.3545454545454545</v>
+        <v>0.3545454545454544</v>
       </c>
       <c r="O25">
-        <v>0.4540909090909092</v>
+        <v>0.454090909090909</v>
       </c>
       <c r="P25">
-        <v>0.0531818181818182</v>
+        <v>0.05318181818181819</v>
       </c>
       <c r="Q25">
-        <v>0.4390909090909092</v>
+        <v>0.4390909090909091</v>
       </c>
       <c r="R25">
         <v>0.6004545454545456</v>
       </c>
       <c r="S25">
-        <v>0.8454545454545453</v>
+        <v>0.8454545454545456</v>
       </c>
       <c r="T25">
         <v>0.025</v>
@@ -2949,34 +2943,34 @@
         <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G26" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K26" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="L26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M26">
         <v>38</v>
@@ -2994,7 +2988,7 @@
         <v>0.468</v>
       </c>
       <c r="R26">
-        <v>0.75</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="S26">
         <v>0.215</v>
@@ -3011,34 +3005,34 @@
         <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K27" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M27">
         <v>42</v>
@@ -3073,34 +3067,34 @@
         <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K28" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L28" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M28">
         <v>138</v>
@@ -3109,19 +3103,19 @@
         <v>0.1430769230769231</v>
       </c>
       <c r="O28">
-        <v>0.673846153846154</v>
+        <v>0.6738461538461539</v>
       </c>
       <c r="P28">
-        <v>0.1776923076923076</v>
+        <v>0.1776923076923077</v>
       </c>
       <c r="Q28">
-        <v>0.4015384615384615</v>
+        <v>0.4015384615384616</v>
       </c>
       <c r="R28">
-        <v>0.6653846153846152</v>
+        <v>0.6653846153846155</v>
       </c>
       <c r="S28">
-        <v>0.2269230769230769</v>
+        <v>0.226923076923077</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -3135,34 +3129,34 @@
         <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K29" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M29">
         <v>104</v>
@@ -3197,34 +3191,34 @@
         <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K30" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L30" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M30">
         <v>37</v>
@@ -3242,7 +3236,7 @@
         <v>0.2735714285714286</v>
       </c>
       <c r="R30">
-        <v>0.4485714285714286</v>
+        <v>0.4485714285714285</v>
       </c>
       <c r="S30">
         <v>0.1392857142857143</v>
@@ -3259,34 +3253,34 @@
         <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L31" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M31">
         <v>88</v>
@@ -3304,7 +3298,7 @@
         <v>0.3391666666666667</v>
       </c>
       <c r="R31">
-        <v>0.5966666666666667</v>
+        <v>0.5966666666666668</v>
       </c>
       <c r="S31">
         <v>0.2291666666666667</v>
@@ -3321,31 +3315,31 @@
         <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L32" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M32">
         <v>16</v>
@@ -3360,13 +3354,13 @@
         <v>0.1152941176470588</v>
       </c>
       <c r="Q32">
-        <v>0.49</v>
+        <v>0.4900000000000001</v>
       </c>
       <c r="R32">
-        <v>0.8088235294117645</v>
+        <v>0.8088235294117646</v>
       </c>
       <c r="S32">
-        <v>0.1870588235294118</v>
+        <v>0.1870588235294117</v>
       </c>
       <c r="T32">
         <v>0.1252941176470588</v>
@@ -3374,37 +3368,37 @@
     </row>
     <row r="33" spans="1:20">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
         <v>107</v>
       </c>
       <c r="C33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L33" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M33">
         <v>43</v>
@@ -3422,7 +3416,7 @@
         <v>0.1627272727272727</v>
       </c>
       <c r="R33">
-        <v>0.4745454545454545</v>
+        <v>0.4745454545454546</v>
       </c>
       <c r="S33">
         <v>0.2609090909090909</v>
@@ -3439,34 +3433,34 @@
         <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L34" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M34">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N34">
         <v>0.1630769230769231</v>
@@ -3475,13 +3469,13 @@
         <v>0.5023076923076922</v>
       </c>
       <c r="P34">
-        <v>0.05692307692307694</v>
+        <v>0.05692307692307692</v>
       </c>
       <c r="Q34">
         <v>0.4846153846153846</v>
       </c>
       <c r="R34">
-        <v>0.7061538461538461</v>
+        <v>0.7061538461538462</v>
       </c>
       <c r="S34">
         <v>0.1623076923076923</v>
@@ -3492,37 +3486,37 @@
     </row>
     <row r="35" spans="1:20">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
         <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J35" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L35" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M35">
         <v>9</v>
@@ -3531,7 +3525,7 @@
         <v>0.344</v>
       </c>
       <c r="O35">
-        <v>0.5713333333333332</v>
+        <v>0.5713333333333334</v>
       </c>
       <c r="P35">
         <v>0.306</v>
@@ -3557,52 +3551,52 @@
         <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L36" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M36">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N36">
         <v>0.4218750000000001</v>
       </c>
       <c r="O36">
-        <v>0.555</v>
+        <v>0.5550000000000002</v>
       </c>
       <c r="P36">
         <v>0.135</v>
       </c>
       <c r="Q36">
-        <v>0.40125</v>
+        <v>0.4012499999999999</v>
       </c>
       <c r="R36">
-        <v>0.4637499999999999</v>
+        <v>0.46375</v>
       </c>
       <c r="S36">
-        <v>0.29125</v>
+        <v>0.2912500000000001</v>
       </c>
       <c r="T36">
         <v>0.17</v>
@@ -3616,31 +3610,31 @@
         <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E37" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J37" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M37">
         <v>81</v>
@@ -3658,13 +3652,13 @@
         <v>0.359375</v>
       </c>
       <c r="R37">
-        <v>0.603125</v>
+        <v>0.6031249999999999</v>
       </c>
       <c r="S37">
         <v>0.1725</v>
       </c>
       <c r="T37">
-        <v>0.46625</v>
+        <v>0.4662500000000001</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -3675,31 +3669,31 @@
         <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L38" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M38">
         <v>27</v>
@@ -3734,31 +3728,31 @@
         <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I39" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L39" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M39">
         <v>51</v>
@@ -3767,7 +3761,7 @@
         <v>0.3642857142857143</v>
       </c>
       <c r="O39">
-        <v>0.5785714285714286</v>
+        <v>0.5785714285714285</v>
       </c>
       <c r="P39">
         <v>0.4185714285714285</v>
@@ -3793,31 +3787,31 @@
         <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G40" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H40" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L40" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M40">
         <v>52</v>
@@ -3829,7 +3823,7 @@
         <v>0.3317857142857142</v>
       </c>
       <c r="P40">
-        <v>0.03857142857142859</v>
+        <v>0.03857142857142858</v>
       </c>
       <c r="Q40">
         <v>0.36</v>
@@ -3838,7 +3832,7 @@
         <v>0.7957142857142857</v>
       </c>
       <c r="S40">
-        <v>0.1789285714285715</v>
+        <v>0.1789285714285714</v>
       </c>
       <c r="T40">
         <v>0.6325000000000001</v>
@@ -3852,55 +3846,55 @@
         <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E41" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L41" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M41">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="N41">
-        <v>0.00125</v>
+        <v>0.07916666666666666</v>
       </c>
       <c r="O41">
-        <v>0.355</v>
+        <v>0.4216666666666667</v>
       </c>
       <c r="P41">
-        <v>0.07375000000000001</v>
+        <v>0.04750000000000001</v>
       </c>
       <c r="Q41">
-        <v>0.415</v>
+        <v>0.4374999999999999</v>
       </c>
       <c r="R41">
-        <v>0.9662499999999999</v>
+        <v>0.71</v>
       </c>
       <c r="S41">
-        <v>0.2525</v>
+        <v>0.1908333333333333</v>
       </c>
       <c r="T41">
-        <v>0.12875</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -3911,55 +3905,55 @@
         <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F42" t="s">
         <v>218</v>
       </c>
       <c r="G42" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H42" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L42" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M42">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N42">
-        <v>0.2845454545454546</v>
+        <v>0.00125</v>
       </c>
       <c r="O42">
-        <v>0.6463636363636364</v>
+        <v>0.355</v>
       </c>
       <c r="P42">
-        <v>0.04545454545454546</v>
+        <v>0.07375000000000001</v>
       </c>
       <c r="Q42">
-        <v>0.71</v>
+        <v>0.415</v>
       </c>
       <c r="R42">
-        <v>0.5918181818181819</v>
+        <v>0.9662499999999999</v>
       </c>
       <c r="S42">
-        <v>0.12</v>
+        <v>0.2525</v>
       </c>
       <c r="T42">
-        <v>0.04909090909090909</v>
+        <v>0.12875</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -3970,55 +3964,55 @@
         <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D43" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="E43" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F43" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G43" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H43" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L43" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M43">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="N43">
-        <v>0.07916666666666666</v>
+        <v>0.2845454545454545</v>
       </c>
       <c r="O43">
-        <v>0.4216666666666667</v>
+        <v>0.6463636363636364</v>
       </c>
       <c r="P43">
-        <v>0.04750000000000001</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="Q43">
-        <v>0.4374999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="R43">
-        <v>0.71</v>
+        <v>0.5918181818181818</v>
       </c>
       <c r="S43">
-        <v>0.1908333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="T43">
-        <v>0.01333333333333333</v>
+        <v>0.04909090909090909</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -4029,55 +4023,55 @@
         <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E44" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G44" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H44" t="s">
         <v>218</v>
       </c>
       <c r="I44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J44" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L44" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M44">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="N44">
-        <v>0.189</v>
+        <v>0.139</v>
       </c>
       <c r="O44">
-        <v>0.612</v>
+        <v>0.371</v>
       </c>
       <c r="P44">
-        <v>0.08400000000000001</v>
+        <v>0.03300000000000001</v>
       </c>
       <c r="Q44">
-        <v>0.398</v>
+        <v>0.2919999999999999</v>
       </c>
       <c r="R44">
-        <v>0.611</v>
+        <v>0.6059999999999999</v>
       </c>
       <c r="S44">
-        <v>0.176</v>
+        <v>0.186</v>
       </c>
       <c r="T44">
-        <v>0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -4088,55 +4082,55 @@
         <v>119</v>
       </c>
       <c r="C45" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D45" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="E45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F45" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G45" t="s">
         <v>220</v>
       </c>
       <c r="H45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J45" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L45" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M45">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="N45">
-        <v>0.139</v>
+        <v>0.3684615384615384</v>
       </c>
       <c r="O45">
-        <v>0.371</v>
+        <v>0.3138461538461538</v>
       </c>
       <c r="P45">
-        <v>0.03300000000000001</v>
+        <v>0.04076923076923077</v>
       </c>
       <c r="Q45">
-        <v>0.2919999999999999</v>
+        <v>0.1638461538461538</v>
       </c>
       <c r="R45">
-        <v>0.6059999999999999</v>
+        <v>0.4584615384615384</v>
       </c>
       <c r="S45">
-        <v>0.186</v>
+        <v>0.3176923076923077</v>
       </c>
       <c r="T45">
-        <v>0.13</v>
+        <v>0.6900000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -4147,55 +4141,55 @@
         <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E46" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="F46" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H46" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J46" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L46" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M46">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="N46">
-        <v>0.3684615384615384</v>
+        <v>0.2809090909090909</v>
       </c>
       <c r="O46">
-        <v>0.3138461538461538</v>
+        <v>0.5345454545454547</v>
       </c>
       <c r="P46">
-        <v>0.04076923076923077</v>
+        <v>0.03000000000000001</v>
       </c>
       <c r="Q46">
-        <v>0.1638461538461538</v>
+        <v>0.3318181818181818</v>
       </c>
       <c r="R46">
-        <v>0.4584615384615385</v>
+        <v>0.5536363636363636</v>
       </c>
       <c r="S46">
-        <v>0.3176923076923077</v>
+        <v>0.1790909090909091</v>
       </c>
       <c r="T46">
-        <v>0.6900000000000002</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -4206,55 +4200,55 @@
         <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E47" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="F47" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G47" t="s">
         <v>220</v>
       </c>
       <c r="H47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L47" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M47">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="N47">
-        <v>0.2809090909090909</v>
+        <v>0.03272727272727273</v>
       </c>
       <c r="O47">
-        <v>0.5345454545454547</v>
+        <v>0.5136363636363636</v>
       </c>
       <c r="P47">
-        <v>0.03000000000000001</v>
+        <v>0.03545454545454545</v>
       </c>
       <c r="Q47">
-        <v>0.3318181818181818</v>
+        <v>0.6927272727272729</v>
       </c>
       <c r="R47">
-        <v>0.5536363636363636</v>
+        <v>0.7836363636363636</v>
       </c>
       <c r="S47">
-        <v>0.1790909090909091</v>
+        <v>0.1645454545454546</v>
       </c>
       <c r="T47">
-        <v>0.09</v>
+        <v>0.2654545454545455</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -4265,55 +4259,55 @@
         <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="E48" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F48" t="s">
         <v>218</v>
       </c>
       <c r="G48" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H48" t="s">
         <v>218</v>
       </c>
       <c r="I48" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L48" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M48">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="N48">
-        <v>0.03272727272727273</v>
+        <v>0.0375</v>
       </c>
       <c r="O48">
-        <v>0.5136363636363637</v>
+        <v>0.3458333333333333</v>
       </c>
       <c r="P48">
-        <v>0.03545454545454545</v>
+        <v>0.08916666666666666</v>
       </c>
       <c r="Q48">
-        <v>0.6927272727272727</v>
+        <v>0.3008333333333333</v>
       </c>
       <c r="R48">
-        <v>0.7836363636363634</v>
+        <v>0.8775000000000001</v>
       </c>
       <c r="S48">
-        <v>0.1645454545454546</v>
+        <v>0.1566666666666667</v>
       </c>
       <c r="T48">
-        <v>0.2654545454545454</v>
+        <v>0.1525</v>
       </c>
     </row>
     <row r="49" spans="1:20">
@@ -4324,55 +4318,55 @@
         <v>123</v>
       </c>
       <c r="C49" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E49" t="s">
         <v>205</v>
       </c>
       <c r="F49" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G49" t="s">
         <v>219</v>
       </c>
       <c r="H49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J49" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L49" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M49">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="N49">
-        <v>0.0375</v>
+        <v>0.24</v>
       </c>
       <c r="O49">
-        <v>0.3458333333333334</v>
+        <v>0.5141666666666668</v>
       </c>
       <c r="P49">
-        <v>0.08916666666666667</v>
+        <v>0.04250000000000001</v>
       </c>
       <c r="Q49">
-        <v>0.3008333333333333</v>
+        <v>0.4125</v>
       </c>
       <c r="R49">
-        <v>0.8774999999999999</v>
+        <v>0.7316666666666665</v>
       </c>
       <c r="S49">
-        <v>0.1566666666666667</v>
+        <v>0.23</v>
       </c>
       <c r="T49">
-        <v>0.1525</v>
+        <v>0.4483333333333334</v>
       </c>
     </row>
     <row r="50" spans="1:20">
@@ -4383,55 +4377,55 @@
         <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E50" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="F50" t="s">
         <v>218</v>
       </c>
       <c r="G50" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L50" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M50">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N50">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="O50">
-        <v>0.5141666666666667</v>
+        <v>0.42125</v>
       </c>
       <c r="P50">
-        <v>0.04250000000000001</v>
+        <v>0.06749999999999999</v>
       </c>
       <c r="Q50">
-        <v>0.4125</v>
+        <v>0.4225</v>
       </c>
       <c r="R50">
-        <v>0.7316666666666665</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="S50">
-        <v>0.23</v>
+        <v>0.1425</v>
       </c>
       <c r="T50">
-        <v>0.4483333333333334</v>
+        <v>0.5075</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -4442,55 +4436,55 @@
         <v>125</v>
       </c>
       <c r="C51" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D51" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E51" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G51" t="s">
         <v>219</v>
       </c>
       <c r="H51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I51" t="s">
         <v>236</v>
       </c>
       <c r="J51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L51" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M51">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="N51">
-        <v>0</v>
+        <v>0.1305882352941176</v>
       </c>
       <c r="O51">
-        <v>0.42125</v>
+        <v>0.6858823529411765</v>
       </c>
       <c r="P51">
-        <v>0.0675</v>
+        <v>0.09411764705882354</v>
       </c>
       <c r="Q51">
-        <v>0.4225</v>
+        <v>0.3176470588235295</v>
       </c>
       <c r="R51">
-        <v>0.8149999999999999</v>
+        <v>0.6388235294117649</v>
       </c>
       <c r="S51">
-        <v>0.1425</v>
+        <v>0.1905882352941177</v>
       </c>
       <c r="T51">
-        <v>0.5075</v>
+        <v>0.0005882352941176471</v>
       </c>
     </row>
     <row r="52" spans="1:20">
@@ -4501,55 +4495,55 @@
         <v>126</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D52" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="E52" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F52" t="s">
+        <v>218</v>
+      </c>
+      <c r="G52" t="s">
         <v>219</v>
       </c>
-      <c r="G52" t="s">
-        <v>220</v>
-      </c>
       <c r="H52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J52" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L52" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M52">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="N52">
-        <v>0.1305882352941176</v>
+        <v>0</v>
       </c>
       <c r="O52">
-        <v>0.6858823529411765</v>
+        <v>0.32875</v>
       </c>
       <c r="P52">
-        <v>0.09411764705882354</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Q52">
-        <v>0.3176470588235294</v>
+        <v>0.16875</v>
       </c>
       <c r="R52">
-        <v>0.6388235294117648</v>
+        <v>0.9224999999999999</v>
       </c>
       <c r="S52">
-        <v>0.1905882352941177</v>
+        <v>0.1875</v>
       </c>
       <c r="T52">
-        <v>0.0005882352941176471</v>
+        <v>0.8724999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:20">
@@ -4560,55 +4554,55 @@
         <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="E53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F53" t="s">
+        <v>218</v>
+      </c>
+      <c r="G53" t="s">
         <v>219</v>
       </c>
-      <c r="G53" t="s">
-        <v>220</v>
-      </c>
       <c r="H53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I53" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J53" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L53" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M53">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>0.1657142857142857</v>
       </c>
       <c r="O53">
-        <v>0.32875</v>
+        <v>0.6671428571428571</v>
       </c>
       <c r="P53">
-        <v>0.07000000000000001</v>
+        <v>0.08785714285714288</v>
       </c>
       <c r="Q53">
-        <v>0.16875</v>
+        <v>0.4392857142857143</v>
       </c>
       <c r="R53">
-        <v>0.9225</v>
+        <v>0.6178571428571429</v>
       </c>
       <c r="S53">
-        <v>0.1875</v>
+        <v>0.1878571428571429</v>
       </c>
       <c r="T53">
-        <v>0.8724999999999999</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="54" spans="1:20">
@@ -4619,90 +4613,90 @@
         <v>128</v>
       </c>
       <c r="C54" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D54" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="E54" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G54" t="s">
         <v>220</v>
       </c>
       <c r="H54" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I54" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J54" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L54" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M54">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="N54">
-        <v>0.2471428571428572</v>
+        <v>0.189</v>
       </c>
       <c r="O54">
-        <v>0.6471428571428571</v>
+        <v>0.612</v>
       </c>
       <c r="P54">
-        <v>0.1185714285714286</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="Q54">
-        <v>0.3785714285714286</v>
+        <v>0.398</v>
       </c>
       <c r="R54">
-        <v>0.6214285714285713</v>
+        <v>0.6109999999999999</v>
       </c>
       <c r="S54">
-        <v>0.2142857142857143</v>
+        <v>0.176</v>
       </c>
       <c r="T54">
-        <v>0.005714285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:20">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
         <v>129</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D55" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F55" t="s">
+        <v>218</v>
+      </c>
+      <c r="G55" t="s">
         <v>219</v>
       </c>
-      <c r="G55" t="s">
-        <v>220</v>
-      </c>
       <c r="H55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I55" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L55" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M55">
         <v>8</v>
@@ -4711,16 +4705,16 @@
         <v>0.195</v>
       </c>
       <c r="O55">
-        <v>0.6533333333333333</v>
+        <v>0.6533333333333332</v>
       </c>
       <c r="P55">
-        <v>0.2758333333333334</v>
+        <v>0.2758333333333333</v>
       </c>
       <c r="Q55">
         <v>0.4858333333333333</v>
       </c>
       <c r="R55">
-        <v>0.5666666666666667</v>
+        <v>0.5666666666666665</v>
       </c>
       <c r="S55">
         <v>0.2341666666666667</v>
@@ -4737,34 +4731,34 @@
         <v>130</v>
       </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D56" t="s">
         <v>184</v>
       </c>
       <c r="E56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L56" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M56">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="N56">
         <v>0.4383333333333333</v>
@@ -4779,7 +4773,7 @@
         <v>0.1466666666666666</v>
       </c>
       <c r="R56">
-        <v>0.5191666666666668</v>
+        <v>0.5191666666666667</v>
       </c>
       <c r="S56">
         <v>0.1333333333333333</v>
@@ -4796,31 +4790,31 @@
         <v>131</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F57" t="s">
+        <v>218</v>
+      </c>
+      <c r="G57" t="s">
         <v>219</v>
       </c>
-      <c r="G57" t="s">
-        <v>220</v>
-      </c>
       <c r="H57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J57" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L57" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M57">
         <v>18</v>
@@ -4829,7 +4823,7 @@
         <v>0.6736363636363637</v>
       </c>
       <c r="O57">
-        <v>0.4254545454545454</v>
+        <v>0.4254545454545455</v>
       </c>
       <c r="P57">
         <v>0.03363636363636364</v>
@@ -4855,55 +4849,55 @@
         <v>132</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D58" t="s">
         <v>185</v>
       </c>
       <c r="E58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G58" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J58" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L58" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M58">
         <v>8</v>
       </c>
       <c r="N58">
-        <v>0.03333333333333334</v>
+        <v>0.1569230769230769</v>
       </c>
       <c r="O58">
-        <v>0.4233333333333333</v>
+        <v>0.4415384615384615</v>
       </c>
       <c r="P58">
-        <v>0.04777777777777778</v>
+        <v>0.04538461538461538</v>
       </c>
       <c r="Q58">
-        <v>0.1533333333333333</v>
+        <v>0.1484615384615385</v>
       </c>
       <c r="R58">
-        <v>0.7255555555555556</v>
+        <v>0.653846153846154</v>
       </c>
       <c r="S58">
-        <v>0.1644444444444445</v>
+        <v>0.1453846153846154</v>
       </c>
       <c r="T58">
-        <v>0.27</v>
+        <v>0.2423076923076923</v>
       </c>
     </row>
     <row r="59" spans="1:20">
@@ -4914,31 +4908,31 @@
         <v>133</v>
       </c>
       <c r="C59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D59" t="s">
         <v>177</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F59" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G59" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H59" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I59" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J59" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L59" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M59">
         <v>11</v>
@@ -4973,31 +4967,31 @@
         <v>134</v>
       </c>
       <c r="C60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E60" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F60" t="s">
+        <v>218</v>
+      </c>
+      <c r="G60" t="s">
         <v>219</v>
       </c>
-      <c r="G60" t="s">
-        <v>220</v>
-      </c>
       <c r="H60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J60" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L60" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M60">
         <v>71</v>
@@ -5032,31 +5026,31 @@
         <v>135</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D61" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E61" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J61" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L61" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M61">
         <v>20</v>
@@ -5071,7 +5065,7 @@
         <v>0.05928571428571429</v>
       </c>
       <c r="Q61">
-        <v>0.5785714285714286</v>
+        <v>0.5785714285714285</v>
       </c>
       <c r="R61">
         <v>0.8757142857142857</v>
@@ -5091,37 +5085,37 @@
         <v>136</v>
       </c>
       <c r="C62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D62" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F62" t="s">
+        <v>219</v>
+      </c>
+      <c r="G62" t="s">
+        <v>216</v>
+      </c>
+      <c r="H62" t="s">
         <v>220</v>
       </c>
-      <c r="G62" t="s">
-        <v>217</v>
-      </c>
-      <c r="H62" t="s">
-        <v>221</v>
-      </c>
       <c r="I62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L62" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M62">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N62">
-        <v>0.3599999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="O62">
         <v>0.481</v>
@@ -5133,7 +5127,7 @@
         <v>0.445</v>
       </c>
       <c r="R62">
-        <v>0.457</v>
+        <v>0.4570000000000001</v>
       </c>
       <c r="S62">
         <v>0.138</v>
@@ -5150,31 +5144,31 @@
         <v>137</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E63" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F63" t="s">
+        <v>218</v>
+      </c>
+      <c r="G63" t="s">
+        <v>218</v>
+      </c>
+      <c r="H63" t="s">
         <v>219</v>
       </c>
-      <c r="G63" t="s">
-        <v>219</v>
-      </c>
-      <c r="H63" t="s">
-        <v>220</v>
-      </c>
       <c r="I63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J63" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L63" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M63">
         <v>29</v>
@@ -5183,13 +5177,13 @@
         <v>0.3953846153846153</v>
       </c>
       <c r="O63">
-        <v>0.51</v>
+        <v>0.5099999999999999</v>
       </c>
       <c r="P63">
         <v>0.1030769230769231</v>
       </c>
       <c r="Q63">
-        <v>0.4407692307692308</v>
+        <v>0.4407692307692307</v>
       </c>
       <c r="R63">
         <v>0.5207692307692308</v>
@@ -5209,37 +5203,37 @@
         <v>138</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D64" t="s">
         <v>186</v>
       </c>
       <c r="E64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G64" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J64" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L64" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M64">
         <v>4</v>
       </c>
       <c r="N64">
-        <v>0.05</v>
+        <v>0.05000000000000001</v>
       </c>
       <c r="O64">
         <v>0.4961538461538462</v>
@@ -5248,13 +5242,13 @@
         <v>0.09769230769230772</v>
       </c>
       <c r="Q64">
-        <v>0.4684615384615384</v>
+        <v>0.4684615384615385</v>
       </c>
       <c r="R64">
         <v>0.8761538461538461</v>
       </c>
       <c r="S64">
-        <v>0.2507692307692307</v>
+        <v>0.2507692307692308</v>
       </c>
       <c r="T64">
         <v>0.1323076923076923</v>
@@ -5268,40 +5262,40 @@
         <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D65" t="s">
         <v>186</v>
       </c>
       <c r="E65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F65" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G65" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H65" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I65" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J65" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L65" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M65">
         <v>3</v>
       </c>
       <c r="N65">
-        <v>0.05200000000000001</v>
+        <v>0.052</v>
       </c>
       <c r="O65">
-        <v>0.5653333333333332</v>
+        <v>0.5653333333333334</v>
       </c>
       <c r="P65">
         <v>0.1246666666666667</v>
@@ -5327,31 +5321,31 @@
         <v>140</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D66" t="s">
         <v>187</v>
       </c>
       <c r="E66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G66" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J66" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L66" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M66">
         <v>11</v>
@@ -5360,7 +5354,7 @@
         <v>0.1045454545454546</v>
       </c>
       <c r="O66">
-        <v>0.6045454545454547</v>
+        <v>0.6045454545454546</v>
       </c>
       <c r="P66">
         <v>0.04545454545454546</v>
@@ -5375,42 +5369,42 @@
         <v>0.1172727272727273</v>
       </c>
       <c r="T66">
-        <v>0.6099999999999999</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="67" spans="1:20">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B67" t="s">
         <v>141</v>
       </c>
       <c r="C67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E67" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F67" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G67" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H67" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I67" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J67" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L67" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M67">
         <v>7</v>
@@ -5422,7 +5416,7 @@
         <v>0.3718181818181818</v>
       </c>
       <c r="P67">
-        <v>0.03272727272727272</v>
+        <v>0.03272727272727273</v>
       </c>
       <c r="Q67">
         <v>0.2463636363636364</v>
@@ -5431,7 +5425,7 @@
         <v>0.6590909090909091</v>
       </c>
       <c r="S67">
-        <v>0.1745454545454545</v>
+        <v>0.1745454545454546</v>
       </c>
       <c r="T67">
         <v>0.7663636363636364</v>
@@ -5445,31 +5439,31 @@
         <v>142</v>
       </c>
       <c r="C68" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D68" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E68" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F68" t="s">
+        <v>218</v>
+      </c>
+      <c r="G68" t="s">
         <v>219</v>
       </c>
-      <c r="G68" t="s">
-        <v>220</v>
-      </c>
       <c r="H68" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J68" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L68" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M68">
         <v>7</v>
@@ -5504,31 +5498,31 @@
         <v>143</v>
       </c>
       <c r="C69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G69" t="s">
+        <v>218</v>
+      </c>
+      <c r="H69" t="s">
         <v>219</v>
       </c>
-      <c r="H69" t="s">
-        <v>220</v>
-      </c>
       <c r="I69" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J69" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L69" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M69">
         <v>15</v>
@@ -5537,7 +5531,7 @@
         <v>0.2142857142857143</v>
       </c>
       <c r="O69">
-        <v>0.5349999999999999</v>
+        <v>0.535</v>
       </c>
       <c r="P69">
         <v>0.05571428571428572</v>
@@ -5546,7 +5540,7 @@
         <v>0.29</v>
       </c>
       <c r="R69">
-        <v>0.5200000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="S69">
         <v>0.1814285714285714</v>
@@ -5563,43 +5557,43 @@
         <v>144</v>
       </c>
       <c r="C70" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E70" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J70" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L70" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M70">
         <v>18</v>
       </c>
       <c r="N70">
-        <v>0.6621428571428571</v>
+        <v>0.6621428571428573</v>
       </c>
       <c r="O70">
-        <v>0.4814285714285714</v>
+        <v>0.4814285714285713</v>
       </c>
       <c r="P70">
-        <v>0.04357142857142857</v>
+        <v>0.04357142857142856</v>
       </c>
       <c r="Q70">
         <v>0.205</v>
@@ -5611,7 +5605,7 @@
         <v>0.1278571428571429</v>
       </c>
       <c r="T70">
-        <v>0.2421428571428572</v>
+        <v>0.2421428571428571</v>
       </c>
     </row>
     <row r="71" spans="1:20">
@@ -5622,31 +5616,31 @@
         <v>145</v>
       </c>
       <c r="C71" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H71" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L71" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M71">
         <v>4</v>
@@ -5658,13 +5652,13 @@
         <v>0.46875</v>
       </c>
       <c r="P71">
-        <v>0.04875</v>
+        <v>0.04875000000000001</v>
       </c>
       <c r="Q71">
         <v>0.405</v>
       </c>
       <c r="R71">
-        <v>0.7206250000000001</v>
+        <v>0.720625</v>
       </c>
       <c r="S71">
         <v>0.20625</v>
@@ -5675,7 +5669,7 @@
     </row>
     <row r="72" spans="1:20">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
         <v>146</v>
@@ -5684,110 +5678,51 @@
         <v>148</v>
       </c>
       <c r="D72" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E72" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="F72" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G72" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H72" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J72" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L72" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M72">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="N72">
-        <v>0.1171428571428571</v>
+        <v>0.2921052631578946</v>
       </c>
       <c r="O72">
-        <v>0.5764285714285713</v>
+        <v>0.5021052631578948</v>
       </c>
       <c r="P72">
-        <v>0.1857142857142857</v>
+        <v>0.0468421052631579</v>
       </c>
       <c r="Q72">
-        <v>0.5185714285714286</v>
+        <v>0.4747368421052631</v>
       </c>
       <c r="R72">
-        <v>0.6228571428571428</v>
+        <v>0.5910526315789472</v>
       </c>
       <c r="S72">
-        <v>0.3</v>
+        <v>0.2057894736842105</v>
       </c>
       <c r="T72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20">
-      <c r="A73" t="s">
-        <v>75</v>
-      </c>
-      <c r="B73" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" t="s">
-        <v>149</v>
-      </c>
-      <c r="D73" t="s">
-        <v>168</v>
-      </c>
-      <c r="E73" t="s">
-        <v>205</v>
-      </c>
-      <c r="F73" t="s">
-        <v>221</v>
-      </c>
-      <c r="G73" t="s">
-        <v>217</v>
-      </c>
-      <c r="H73" t="s">
-        <v>221</v>
-      </c>
-      <c r="I73" t="s">
-        <v>238</v>
-      </c>
-      <c r="J73" t="s">
-        <v>310</v>
-      </c>
-      <c r="L73" t="s">
-        <v>337</v>
-      </c>
-      <c r="M73">
-        <v>5</v>
-      </c>
-      <c r="N73">
-        <v>0.2921052631578947</v>
-      </c>
-      <c r="O73">
-        <v>0.5021052631578947</v>
-      </c>
-      <c r="P73">
-        <v>0.04684210526315791</v>
-      </c>
-      <c r="Q73">
-        <v>0.4747368421052632</v>
-      </c>
-      <c r="R73">
-        <v>0.5910526315789473</v>
-      </c>
-      <c r="S73">
-        <v>0.2057894736842105</v>
-      </c>
-      <c r="T73">
         <v>0.1931578947368421</v>
       </c>
     </row>

</xml_diff>

<commit_message>
selenium+bs4 scrapes + lyrics genius done
</commit_message>
<xml_diff>
--- a/exports/Top 100.xlsx
+++ b/exports/Top 100.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="340">
   <si>
     <t>artist</t>
   </si>
@@ -226,6 +226,9 @@
     <t>Bright Eyes</t>
   </si>
   <si>
+    <t>IDLES</t>
+  </si>
+  <si>
     <t>The Unicorns</t>
   </si>
   <si>
@@ -427,6 +430,9 @@
     <t>i'm wide awake, it's morning</t>
   </si>
   <si>
+    <t>joy as an act of resistance</t>
+  </si>
+  <si>
     <t>who will cut our hair when we're gone</t>
   </si>
   <si>
@@ -574,6 +580,9 @@
     <t>Djent</t>
   </si>
   <si>
+    <t>Post Punk</t>
+  </si>
+  <si>
     <t>Nu-Metal</t>
   </si>
   <si>
@@ -911,6 +920,9 @@
   </si>
   <si>
     <t>Lua</t>
+  </si>
+  <si>
+    <t>Never Fight A Man With A Perm</t>
   </si>
   <si>
     <t>Tuff Ghost</t>
@@ -1379,7 +1391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T72"/>
+  <dimension ref="A1:T73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1452,37 +1464,37 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I2" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="K2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="L2" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="M2">
         <v>68</v>
@@ -1497,7 +1509,7 @@
         <v>0.1423076923076923</v>
       </c>
       <c r="Q2">
-        <v>0.3676923076923077</v>
+        <v>0.3676923076923078</v>
       </c>
       <c r="R2">
         <v>0.6861538461538461</v>
@@ -1514,37 +1526,37 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="K3" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="L3" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="M3">
         <v>55</v>
@@ -1576,37 +1588,37 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J4" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="K4" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="L4" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="M4">
         <v>24</v>
@@ -1638,37 +1650,37 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G5" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J5" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="K5" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="L5" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="M5">
         <v>25</v>
@@ -1700,37 +1712,37 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E6" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F6" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G6" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H6" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I6" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="K6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="L6" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="M6">
         <v>212</v>
@@ -1739,7 +1751,7 @@
         <v>0.7185294117647061</v>
       </c>
       <c r="O6">
-        <v>0.501470588235294</v>
+        <v>0.5014705882352941</v>
       </c>
       <c r="P6">
         <v>0.1923529411764706</v>
@@ -1762,37 +1774,37 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F7" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G7" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H7" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I7" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J7" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="K7" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="L7" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="M7">
         <v>3</v>
@@ -1824,37 +1836,37 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F8" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G8" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H8" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I8" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="J8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="K8" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="L8" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="M8">
         <v>32</v>
@@ -1886,37 +1898,37 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F9" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G9" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H9" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I9" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="J9" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="K9" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="L9" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="M9">
         <v>97</v>
@@ -1948,37 +1960,37 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E10" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F10" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="H10" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I10" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="J10" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="K10" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="L10" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="M10">
         <v>30</v>
@@ -2010,37 +2022,37 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F11" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G11" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H11" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I11" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="J11" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="K11" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="L11" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="M11">
         <v>73</v>
@@ -2049,7 +2061,7 @@
         <v>0.7677777777777778</v>
       </c>
       <c r="O11">
-        <v>0.5622222222222223</v>
+        <v>0.5622222222222222</v>
       </c>
       <c r="P11">
         <v>0.05222222222222222</v>
@@ -2072,37 +2084,37 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H12" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I12" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J12" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="K12" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="L12" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M12">
         <v>28</v>
@@ -2134,37 +2146,37 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F13" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G13" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="H13" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I13" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J13" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="K13" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="L13" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M13">
         <v>66</v>
@@ -2173,7 +2185,7 @@
         <v>0.4758333333333333</v>
       </c>
       <c r="O13">
-        <v>0.4099999999999999</v>
+        <v>0.4100000000000001</v>
       </c>
       <c r="P13">
         <v>0.03333333333333333</v>
@@ -2182,7 +2194,7 @@
         <v>0.3425</v>
       </c>
       <c r="R13">
-        <v>0.4308333333333333</v>
+        <v>0.4308333333333334</v>
       </c>
       <c r="S13">
         <v>0.1225</v>
@@ -2196,37 +2208,37 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E14" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F14" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="H14" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I14" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J14" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K14" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="L14" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M14">
         <v>22</v>
@@ -2244,10 +2256,10 @@
         <v>0.36</v>
       </c>
       <c r="R14">
-        <v>0.8014285714285714</v>
+        <v>0.8014285714285715</v>
       </c>
       <c r="S14">
-        <v>0.2064285714285715</v>
+        <v>0.2064285714285714</v>
       </c>
       <c r="T14">
         <v>0.001428571428571429</v>
@@ -2258,37 +2270,37 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F15" t="s">
+        <v>222</v>
+      </c>
+      <c r="G15" t="s">
+        <v>226</v>
+      </c>
+      <c r="H15" t="s">
         <v>219</v>
       </c>
-      <c r="G15" t="s">
-        <v>223</v>
-      </c>
-      <c r="H15" t="s">
-        <v>216</v>
-      </c>
       <c r="I15" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J15" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="K15" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="L15" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M15">
         <v>51</v>
@@ -2320,37 +2332,37 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F16" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G16" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H16" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I16" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J16" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="K16" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="L16" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M16">
         <v>80</v>
@@ -2382,37 +2394,37 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E17" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F17" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G17" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H17" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I17" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J17" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="K17" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="L17" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M17">
         <v>26</v>
@@ -2424,7 +2436,7 @@
         <v>0.5946666666666666</v>
       </c>
       <c r="P17">
-        <v>0.1546666666666666</v>
+        <v>0.1546666666666667</v>
       </c>
       <c r="Q17">
         <v>0.5473333333333333</v>
@@ -2444,37 +2456,37 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E18" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F18" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G18" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="H18" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I18" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J18" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="K18" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="L18" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M18">
         <v>33</v>
@@ -2506,37 +2518,37 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D19" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E19" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F19" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G19" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H19" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I19" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="K19" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="L19" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M19">
         <v>6</v>
@@ -2548,7 +2560,7 @@
         <v>0.6869230769230769</v>
       </c>
       <c r="P19">
-        <v>0.04384615384615385</v>
+        <v>0.04384615384615383</v>
       </c>
       <c r="Q19">
         <v>0.4876923076923077</v>
@@ -2568,37 +2580,37 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F20" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G20" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H20" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I20" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J20" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="K20" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="L20" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M20">
         <v>80</v>
@@ -2630,37 +2642,37 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E21" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F21" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G21" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="H21" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I21" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J21" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="K21" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="L21" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M21">
         <v>59</v>
@@ -2669,16 +2681,16 @@
         <v>0.5454545454545454</v>
       </c>
       <c r="O21">
-        <v>0.5363636363636364</v>
+        <v>0.5363636363636363</v>
       </c>
       <c r="P21">
-        <v>0.03090909090909092</v>
+        <v>0.03090909090909091</v>
       </c>
       <c r="Q21">
         <v>0.2827272727272728</v>
       </c>
       <c r="R21">
-        <v>0.4136363636363637</v>
+        <v>0.4136363636363636</v>
       </c>
       <c r="S21">
         <v>0.17</v>
@@ -2692,37 +2704,37 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E22" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F22" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G22" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H22" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I22" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J22" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="K22" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="L22" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M22">
         <v>87</v>
@@ -2734,13 +2746,13 @@
         <v>0.4615384615384616</v>
       </c>
       <c r="P22">
-        <v>0.0953846153846154</v>
+        <v>0.09538461538461539</v>
       </c>
       <c r="Q22">
         <v>0.4392307692307693</v>
       </c>
       <c r="R22">
-        <v>0.8461538461538461</v>
+        <v>0.8461538461538463</v>
       </c>
       <c r="S22">
         <v>0.1876923076923077</v>
@@ -2754,37 +2766,37 @@
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E23" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F23" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G23" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H23" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I23" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J23" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="K23" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="L23" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M23">
         <v>14</v>
@@ -2816,37 +2828,37 @@
         <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E24" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F24" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G24" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H24" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I24" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J24" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="K24" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="L24" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M24">
         <v>113</v>
@@ -2861,7 +2873,7 @@
         <v>0.04600000000000001</v>
       </c>
       <c r="Q24">
-        <v>0.6133333333333332</v>
+        <v>0.6133333333333333</v>
       </c>
       <c r="R24">
         <v>0.6093333333333334</v>
@@ -2878,37 +2890,37 @@
         <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F25" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G25" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H25" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I25" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J25" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="K25" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="L25" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="M25">
         <v>14</v>
@@ -2940,37 +2952,37 @@
         <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D26" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E26" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F26" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G26" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H26" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I26" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J26" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="K26" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="L26" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="M26">
         <v>38</v>
@@ -2979,7 +2991,7 @@
         <v>0.189</v>
       </c>
       <c r="O26">
-        <v>0.403</v>
+        <v>0.4029999999999999</v>
       </c>
       <c r="P26">
         <v>0.036</v>
@@ -3002,37 +3014,37 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D27" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E27" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F27" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G27" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H27" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I27" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J27" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="K27" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="L27" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="M27">
         <v>42</v>
@@ -3064,37 +3076,37 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D28" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E28" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F28" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G28" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H28" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I28" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J28" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="K28" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="L28" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="M28">
         <v>138</v>
@@ -3106,16 +3118,16 @@
         <v>0.6738461538461539</v>
       </c>
       <c r="P28">
-        <v>0.1776923076923077</v>
+        <v>0.1776923076923076</v>
       </c>
       <c r="Q28">
-        <v>0.4015384615384616</v>
+        <v>0.4015384615384615</v>
       </c>
       <c r="R28">
-        <v>0.6653846153846155</v>
+        <v>0.6653846153846152</v>
       </c>
       <c r="S28">
-        <v>0.226923076923077</v>
+        <v>0.2269230769230769</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -3126,37 +3138,37 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E29" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F29" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G29" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H29" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I29" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J29" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="K29" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="L29" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="M29">
         <v>104</v>
@@ -3165,7 +3177,7 @@
         <v>0.4376666666666666</v>
       </c>
       <c r="O29">
-        <v>0.5433333333333332</v>
+        <v>0.5433333333333333</v>
       </c>
       <c r="P29">
         <v>0.07433333333333335</v>
@@ -3188,37 +3200,37 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D30" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E30" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F30" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G30" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I30" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J30" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="K30" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="L30" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="M30">
         <v>37</v>
@@ -3236,7 +3248,7 @@
         <v>0.2735714285714286</v>
       </c>
       <c r="R30">
-        <v>0.4485714285714285</v>
+        <v>0.4485714285714286</v>
       </c>
       <c r="S30">
         <v>0.1392857142857143</v>
@@ -3250,37 +3262,37 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E31" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F31" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G31" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I31" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J31" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="K31" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="L31" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="M31">
         <v>88</v>
@@ -3298,7 +3310,7 @@
         <v>0.3391666666666667</v>
       </c>
       <c r="R31">
-        <v>0.5966666666666668</v>
+        <v>0.5966666666666667</v>
       </c>
       <c r="S31">
         <v>0.2291666666666667</v>
@@ -3312,34 +3324,34 @@
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F32" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G32" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H32" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I32" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J32" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="L32" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M32">
         <v>16</v>
@@ -3354,7 +3366,7 @@
         <v>0.1152941176470588</v>
       </c>
       <c r="Q32">
-        <v>0.4900000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="R32">
         <v>0.8088235294117646</v>
@@ -3371,34 +3383,34 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E33" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F33" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G33" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H33" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I33" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J33" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="L33" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M33">
         <v>43</v>
@@ -3416,7 +3428,7 @@
         <v>0.1627272727272727</v>
       </c>
       <c r="R33">
-        <v>0.4745454545454546</v>
+        <v>0.4745454545454545</v>
       </c>
       <c r="S33">
         <v>0.2609090909090909</v>
@@ -3430,34 +3442,34 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E34" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F34" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G34" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" t="s">
         <v>220</v>
       </c>
-      <c r="H34" t="s">
-        <v>217</v>
-      </c>
       <c r="I34" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J34" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L34" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M34">
         <v>13</v>
@@ -3489,34 +3501,34 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F35" t="s">
+        <v>222</v>
+      </c>
+      <c r="G35" t="s">
         <v>219</v>
       </c>
-      <c r="G35" t="s">
-        <v>216</v>
-      </c>
       <c r="H35" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I35" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J35" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="L35" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M35">
         <v>9</v>
@@ -3548,43 +3560,43 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D36" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E36" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F36" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G36" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H36" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I36" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J36" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="L36" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M36">
         <v>15</v>
       </c>
       <c r="N36">
-        <v>0.4218750000000001</v>
+        <v>0.421875</v>
       </c>
       <c r="O36">
-        <v>0.5550000000000002</v>
+        <v>0.555</v>
       </c>
       <c r="P36">
         <v>0.135</v>
@@ -3593,10 +3605,10 @@
         <v>0.4012499999999999</v>
       </c>
       <c r="R36">
-        <v>0.46375</v>
+        <v>0.4637499999999999</v>
       </c>
       <c r="S36">
-        <v>0.2912500000000001</v>
+        <v>0.29125</v>
       </c>
       <c r="T36">
         <v>0.17</v>
@@ -3607,34 +3619,34 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D37" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E37" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F37" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G37" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H37" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I37" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J37" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="L37" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M37">
         <v>81</v>
@@ -3658,7 +3670,7 @@
         <v>0.1725</v>
       </c>
       <c r="T37">
-        <v>0.4662500000000001</v>
+        <v>0.46625</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -3666,34 +3678,34 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E38" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F38" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G38" t="s">
+        <v>223</v>
+      </c>
+      <c r="H38" t="s">
         <v>220</v>
       </c>
-      <c r="H38" t="s">
-        <v>217</v>
-      </c>
       <c r="I38" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J38" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L38" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M38">
         <v>27</v>
@@ -3725,34 +3737,34 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E39" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F39" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G39" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H39" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I39" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J39" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="L39" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M39">
         <v>51</v>
@@ -3761,7 +3773,7 @@
         <v>0.3642857142857143</v>
       </c>
       <c r="O39">
-        <v>0.5785714285714285</v>
+        <v>0.5785714285714286</v>
       </c>
       <c r="P39">
         <v>0.4185714285714285</v>
@@ -3784,34 +3796,34 @@
         <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E40" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F40" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G40" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H40" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I40" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J40" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="L40" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M40">
         <v>52</v>
@@ -3823,7 +3835,7 @@
         <v>0.3317857142857142</v>
       </c>
       <c r="P40">
-        <v>0.03857142857142858</v>
+        <v>0.03857142857142859</v>
       </c>
       <c r="Q40">
         <v>0.36</v>
@@ -3843,34 +3855,34 @@
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E41" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F41" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G41" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H41" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I41" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J41" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="L41" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M41">
         <v>68</v>
@@ -3902,34 +3914,34 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E42" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F42" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G42" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H42" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I42" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J42" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="L42" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M42">
         <v>4</v>
@@ -3961,34 +3973,34 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D43" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E43" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F43" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G43" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H43" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I43" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J43" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="L43" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M43">
         <v>15</v>
@@ -4003,7 +4015,7 @@
         <v>0.04545454545454546</v>
       </c>
       <c r="Q43">
-        <v>0.71</v>
+        <v>0.7100000000000001</v>
       </c>
       <c r="R43">
         <v>0.5918181818181818</v>
@@ -4020,34 +4032,34 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D44" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E44" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F44" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G44" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H44" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I44" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J44" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="L44" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M44">
         <v>55</v>
@@ -4079,34 +4091,34 @@
         <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D45" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E45" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F45" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G45" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H45" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I45" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J45" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="L45" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M45">
         <v>32</v>
@@ -4138,34 +4150,34 @@
         <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D46" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E46" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F46" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G46" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H46" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="I46" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J46" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="L46" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M46">
         <v>63</v>
@@ -4197,34 +4209,34 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C47" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E47" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F47" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G47" t="s">
+        <v>223</v>
+      </c>
+      <c r="H47" t="s">
         <v>220</v>
       </c>
-      <c r="H47" t="s">
-        <v>217</v>
-      </c>
       <c r="I47" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J47" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="L47" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M47">
         <v>10</v>
@@ -4256,34 +4268,34 @@
         <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C48" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D48" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E48" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F48" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G48" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H48" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I48" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J48" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="L48" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M48">
         <v>21</v>
@@ -4292,7 +4304,7 @@
         <v>0.0375</v>
       </c>
       <c r="O48">
-        <v>0.3458333333333333</v>
+        <v>0.3458333333333334</v>
       </c>
       <c r="P48">
         <v>0.08916666666666666</v>
@@ -4315,34 +4327,34 @@
         <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D49" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E49" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F49" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G49" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H49" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I49" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J49" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="L49" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M49">
         <v>7</v>
@@ -4374,34 +4386,34 @@
         <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D50" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E50" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F50" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G50" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H50" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I50" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J50" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="L50" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="M50">
         <v>0</v>
@@ -4433,34 +4445,34 @@
         <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D51" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E51" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F51" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G51" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H51" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I51" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J51" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="L51" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M51">
         <v>131</v>
@@ -4469,16 +4481,16 @@
         <v>0.1305882352941176</v>
       </c>
       <c r="O51">
-        <v>0.6858823529411765</v>
+        <v>0.6858823529411766</v>
       </c>
       <c r="P51">
         <v>0.09411764705882354</v>
       </c>
       <c r="Q51">
-        <v>0.3176470588235295</v>
+        <v>0.3176470588235294</v>
       </c>
       <c r="R51">
-        <v>0.6388235294117649</v>
+        <v>0.6388235294117648</v>
       </c>
       <c r="S51">
         <v>0.1905882352941177</v>
@@ -4492,34 +4504,34 @@
         <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E52" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F52" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G52" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H52" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I52" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J52" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="L52" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M52">
         <v>45</v>
@@ -4551,37 +4563,37 @@
         <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D53" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E53" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F53" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G53" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H53" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I53" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J53" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="L53" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M53">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="N53">
         <v>0.1657142857142857</v>
@@ -4590,13 +4602,13 @@
         <v>0.6671428571428571</v>
       </c>
       <c r="P53">
-        <v>0.08785714285714288</v>
+        <v>0.08785714285714287</v>
       </c>
       <c r="Q53">
         <v>0.4392857142857143</v>
       </c>
       <c r="R53">
-        <v>0.6178571428571429</v>
+        <v>0.6178571428571428</v>
       </c>
       <c r="S53">
         <v>0.1878571428571429</v>
@@ -4610,34 +4622,34 @@
         <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E54" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F54" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G54" t="s">
+        <v>223</v>
+      </c>
+      <c r="H54" t="s">
         <v>220</v>
       </c>
-      <c r="H54" t="s">
-        <v>217</v>
-      </c>
       <c r="I54" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J54" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="L54" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M54">
         <v>12</v>
@@ -4669,34 +4681,34 @@
         <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C55" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E55" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F55" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G55" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H55" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I55" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J55" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L55" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M55">
         <v>8</v>
@@ -4714,7 +4726,7 @@
         <v>0.4858333333333333</v>
       </c>
       <c r="R55">
-        <v>0.5666666666666665</v>
+        <v>0.5666666666666668</v>
       </c>
       <c r="S55">
         <v>0.2341666666666667</v>
@@ -4728,37 +4740,37 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D56" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E56" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F56" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G56" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H56" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I56" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J56" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="L56" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M56">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N56">
         <v>0.4383333333333333</v>
@@ -4779,7 +4791,7 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="T56">
-        <v>0.5525</v>
+        <v>0.5525000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:20">
@@ -4787,34 +4799,34 @@
         <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C57" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E57" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F57" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G57" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H57" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I57" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J57" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="L57" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M57">
         <v>18</v>
@@ -4846,58 +4858,58 @@
         <v>65</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C58" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D58" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E58" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F58" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G58" t="s">
+        <v>223</v>
+      </c>
+      <c r="H58" t="s">
         <v>220</v>
       </c>
-      <c r="H58" t="s">
-        <v>217</v>
-      </c>
       <c r="I58" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J58" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="L58" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M58">
         <v>8</v>
       </c>
       <c r="N58">
-        <v>0.1569230769230769</v>
+        <v>0.03333333333333334</v>
       </c>
       <c r="O58">
-        <v>0.4415384615384615</v>
+        <v>0.4233333333333333</v>
       </c>
       <c r="P58">
-        <v>0.04538461538461538</v>
+        <v>0.04777777777777778</v>
       </c>
       <c r="Q58">
-        <v>0.1484615384615385</v>
+        <v>0.1533333333333333</v>
       </c>
       <c r="R58">
-        <v>0.653846153846154</v>
+        <v>0.7255555555555556</v>
       </c>
       <c r="S58">
-        <v>0.1453846153846154</v>
+        <v>0.1644444444444445</v>
       </c>
       <c r="T58">
-        <v>0.2423076923076923</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="59" spans="1:20">
@@ -4905,34 +4917,34 @@
         <v>66</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E59" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F59" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G59" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H59" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I59" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J59" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="L59" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M59">
         <v>11</v>
@@ -4964,34 +4976,34 @@
         <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C60" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D60" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E60" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F60" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G60" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H60" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I60" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J60" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="L60" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M60">
         <v>71</v>
@@ -5015,7 +5027,7 @@
         <v>0.2022727272727273</v>
       </c>
       <c r="T60">
-        <v>0.5618181818181817</v>
+        <v>0.5618181818181818</v>
       </c>
     </row>
     <row r="61" spans="1:20">
@@ -5023,37 +5035,37 @@
         <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D61" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E61" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F61" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G61" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H61" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I61" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J61" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="L61" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M61">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N61">
         <v>0.0742857142857143</v>
@@ -5065,7 +5077,7 @@
         <v>0.05928571428571429</v>
       </c>
       <c r="Q61">
-        <v>0.5785714285714285</v>
+        <v>0.5785714285714286</v>
       </c>
       <c r="R61">
         <v>0.8757142857142857</v>
@@ -5082,34 +5094,34 @@
         <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C62" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E62" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F62" t="s">
+        <v>222</v>
+      </c>
+      <c r="G62" t="s">
         <v>219</v>
       </c>
-      <c r="G62" t="s">
-        <v>216</v>
-      </c>
       <c r="H62" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="I62" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J62" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="L62" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M62">
         <v>28</v>
@@ -5141,58 +5153,58 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="E63" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F63" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G63" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H63" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I63" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J63" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="L63" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M63">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N63">
-        <v>0.3953846153846153</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="O63">
-        <v>0.5099999999999999</v>
+        <v>0.3658333333333334</v>
       </c>
       <c r="P63">
-        <v>0.1030769230769231</v>
+        <v>0.09833333333333333</v>
       </c>
       <c r="Q63">
-        <v>0.4407692307692307</v>
+        <v>0.2633333333333334</v>
       </c>
       <c r="R63">
-        <v>0.5207692307692308</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="S63">
-        <v>0.2130769230769231</v>
+        <v>0.2266666666666667</v>
       </c>
       <c r="T63">
-        <v>0.1207692307692308</v>
+        <v>0.05916666666666667</v>
       </c>
     </row>
     <row r="64" spans="1:20">
@@ -5200,117 +5212,117 @@
         <v>71</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C64" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="E64" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F64" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G64" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H64" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I64" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J64" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="L64" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M64">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="N64">
-        <v>0.05000000000000001</v>
+        <v>0.3953846153846153</v>
       </c>
       <c r="O64">
-        <v>0.4961538461538462</v>
+        <v>0.51</v>
       </c>
       <c r="P64">
-        <v>0.09769230769230772</v>
+        <v>0.1030769230769231</v>
       </c>
       <c r="Q64">
-        <v>0.4684615384615385</v>
+        <v>0.4407692307692308</v>
       </c>
       <c r="R64">
-        <v>0.8761538461538461</v>
+        <v>0.5207692307692308</v>
       </c>
       <c r="S64">
-        <v>0.2507692307692308</v>
+        <v>0.2130769230769231</v>
       </c>
       <c r="T64">
-        <v>0.1323076923076923</v>
+        <v>0.1207692307692308</v>
       </c>
     </row>
     <row r="65" spans="1:20">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D65" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E65" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="F65" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G65" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H65" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="I65" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J65" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="L65" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N65">
-        <v>0.052</v>
+        <v>0.05000000000000001</v>
       </c>
       <c r="O65">
-        <v>0.5653333333333334</v>
+        <v>0.4961538461538462</v>
       </c>
       <c r="P65">
-        <v>0.1246666666666667</v>
+        <v>0.09769230769230772</v>
       </c>
       <c r="Q65">
-        <v>0.486</v>
+        <v>0.4684615384615385</v>
       </c>
       <c r="R65">
-        <v>0.8800000000000001</v>
+        <v>0.8761538461538461</v>
       </c>
       <c r="S65">
-        <v>0.29</v>
+        <v>0.2507692307692308</v>
       </c>
       <c r="T65">
-        <v>0.004</v>
+        <v>0.1323076923076923</v>
       </c>
     </row>
     <row r="66" spans="1:20">
@@ -5318,411 +5330,470 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D66" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E66" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="F66" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G66" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H66" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="I66" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J66" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="L66" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M66">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="N66">
-        <v>0.1045454545454546</v>
+        <v>0.052</v>
       </c>
       <c r="O66">
-        <v>0.6045454545454546</v>
+        <v>0.5653333333333334</v>
       </c>
       <c r="P66">
-        <v>0.04545454545454546</v>
+        <v>0.1246666666666667</v>
       </c>
       <c r="Q66">
-        <v>0.36</v>
+        <v>0.486</v>
       </c>
       <c r="R66">
-        <v>0.5381818181818182</v>
+        <v>0.8800000000000001</v>
       </c>
       <c r="S66">
-        <v>0.1172727272727273</v>
+        <v>0.29</v>
       </c>
       <c r="T66">
-        <v>0.61</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="67" spans="1:20">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D67" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="E67" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="F67" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G67" t="s">
+        <v>228</v>
+      </c>
+      <c r="H67" t="s">
         <v>220</v>
       </c>
-      <c r="H67" t="s">
-        <v>218</v>
-      </c>
       <c r="I67" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="J67" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="L67" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M67">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N67">
-        <v>0.3490909090909091</v>
+        <v>0.1045454545454546</v>
       </c>
       <c r="O67">
-        <v>0.3718181818181818</v>
+        <v>0.6045454545454546</v>
       </c>
       <c r="P67">
-        <v>0.03272727272727273</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="Q67">
-        <v>0.2463636363636364</v>
+        <v>0.36</v>
       </c>
       <c r="R67">
-        <v>0.6590909090909091</v>
+        <v>0.5381818181818182</v>
       </c>
       <c r="S67">
-        <v>0.1745454545454546</v>
+        <v>0.1172727272727273</v>
       </c>
       <c r="T67">
-        <v>0.7663636363636364</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="68" spans="1:20">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C68" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E68" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="F68" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G68" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="H68" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I68" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="J68" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="L68" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M68">
         <v>7</v>
       </c>
       <c r="N68">
-        <v>0.271</v>
+        <v>0.3490909090909091</v>
       </c>
       <c r="O68">
-        <v>0.654</v>
+        <v>0.3718181818181818</v>
       </c>
       <c r="P68">
-        <v>0.09500000000000001</v>
+        <v>0.03272727272727273</v>
       </c>
       <c r="Q68">
-        <v>0.5700000000000001</v>
+        <v>0.2463636363636364</v>
       </c>
       <c r="R68">
-        <v>0.548</v>
+        <v>0.6590909090909091</v>
       </c>
       <c r="S68">
-        <v>0.19</v>
+        <v>0.1745454545454545</v>
       </c>
       <c r="T68">
-        <v>0.036</v>
+        <v>0.7663636363636364</v>
       </c>
     </row>
     <row r="69" spans="1:20">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C69" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D69" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="E69" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="F69" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G69" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H69" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I69" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="J69" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="L69" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M69">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="N69">
-        <v>0.2142857142857143</v>
+        <v>0.271</v>
       </c>
       <c r="O69">
-        <v>0.535</v>
+        <v>0.6540000000000001</v>
       </c>
       <c r="P69">
-        <v>0.05571428571428572</v>
+        <v>0.095</v>
       </c>
       <c r="Q69">
-        <v>0.29</v>
+        <v>0.5700000000000001</v>
       </c>
       <c r="R69">
-        <v>0.52</v>
+        <v>0.548</v>
       </c>
       <c r="S69">
-        <v>0.1814285714285714</v>
+        <v>0.19</v>
       </c>
       <c r="T69">
-        <v>0.0007142857142857143</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="70" spans="1:20">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D70" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E70" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="F70" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G70" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H70" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="I70" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="J70" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="L70" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M70">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N70">
-        <v>0.6621428571428573</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="O70">
-        <v>0.4814285714285713</v>
+        <v>0.535</v>
       </c>
       <c r="P70">
-        <v>0.04357142857142856</v>
+        <v>0.05571428571428572</v>
       </c>
       <c r="Q70">
-        <v>0.205</v>
+        <v>0.29</v>
       </c>
       <c r="R70">
-        <v>0.3842857142857143</v>
+        <v>0.52</v>
       </c>
       <c r="S70">
-        <v>0.1278571428571429</v>
+        <v>0.1814285714285714</v>
       </c>
       <c r="T70">
-        <v>0.2421428571428571</v>
+        <v>0.0007142857142857143</v>
       </c>
     </row>
     <row r="71" spans="1:20">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D71" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E71" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="F71" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G71" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="H71" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I71" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="J71" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="L71" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="M71">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="N71">
-        <v>0.2175</v>
+        <v>0.6621428571428573</v>
       </c>
       <c r="O71">
-        <v>0.46875</v>
+        <v>0.4814285714285714</v>
       </c>
       <c r="P71">
-        <v>0.04875000000000001</v>
+        <v>0.04357142857142858</v>
       </c>
       <c r="Q71">
-        <v>0.405</v>
+        <v>0.205</v>
       </c>
       <c r="R71">
-        <v>0.720625</v>
+        <v>0.3842857142857143</v>
       </c>
       <c r="S71">
-        <v>0.20625</v>
+        <v>0.1278571428571429</v>
       </c>
       <c r="T71">
-        <v>0.22375</v>
+        <v>0.2421428571428572</v>
       </c>
     </row>
     <row r="72" spans="1:20">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C72" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" t="s">
+        <v>169</v>
+      </c>
+      <c r="E72" t="s">
+        <v>191</v>
+      </c>
+      <c r="F72" t="s">
+        <v>223</v>
+      </c>
+      <c r="G72" t="s">
+        <v>220</v>
+      </c>
+      <c r="H72" t="s">
+        <v>222</v>
+      </c>
+      <c r="I72" t="s">
+        <v>240</v>
+      </c>
+      <c r="J72" t="s">
+        <v>311</v>
+      </c>
+      <c r="L72" t="s">
+        <v>339</v>
+      </c>
+      <c r="M72">
+        <v>4</v>
+      </c>
+      <c r="N72">
+        <v>0.2175</v>
+      </c>
+      <c r="O72">
+        <v>0.46875</v>
+      </c>
+      <c r="P72">
+        <v>0.04875000000000001</v>
+      </c>
+      <c r="Q72">
+        <v>0.405</v>
+      </c>
+      <c r="R72">
+        <v>0.720625</v>
+      </c>
+      <c r="S72">
+        <v>0.20625</v>
+      </c>
+      <c r="T72">
+        <v>0.22375</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
         <v>148</v>
       </c>
-      <c r="D72" t="s">
-        <v>167</v>
-      </c>
-      <c r="E72" t="s">
-        <v>204</v>
-      </c>
-      <c r="F72" t="s">
-        <v>220</v>
-      </c>
-      <c r="G72" t="s">
-        <v>216</v>
-      </c>
-      <c r="H72" t="s">
-        <v>220</v>
-      </c>
-      <c r="I72" t="s">
-        <v>237</v>
-      </c>
-      <c r="J72" t="s">
-        <v>308</v>
-      </c>
-      <c r="L72" t="s">
-        <v>335</v>
-      </c>
-      <c r="M72">
+      <c r="C73" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" t="s">
+        <v>169</v>
+      </c>
+      <c r="E73" t="s">
+        <v>207</v>
+      </c>
+      <c r="F73" t="s">
+        <v>223</v>
+      </c>
+      <c r="G73" t="s">
+        <v>219</v>
+      </c>
+      <c r="H73" t="s">
+        <v>223</v>
+      </c>
+      <c r="I73" t="s">
+        <v>240</v>
+      </c>
+      <c r="J73" t="s">
+        <v>312</v>
+      </c>
+      <c r="L73" t="s">
+        <v>339</v>
+      </c>
+      <c r="M73">
         <v>5</v>
       </c>
-      <c r="N72">
+      <c r="N73">
         <v>0.2921052631578946</v>
       </c>
-      <c r="O72">
+      <c r="O73">
         <v>0.5021052631578948</v>
       </c>
-      <c r="P72">
+      <c r="P73">
         <v>0.0468421052631579</v>
       </c>
-      <c r="Q72">
+      <c r="Q73">
         <v>0.4747368421052631</v>
       </c>
-      <c r="R72">
+      <c r="R73">
         <v>0.5910526315789472</v>
       </c>
-      <c r="S72">
+      <c r="S73">
         <v>0.2057894736842105</v>
       </c>
-      <c r="T72">
+      <c r="T73">
         <v>0.1931578947368421</v>
       </c>
     </row>

</xml_diff>

<commit_message>
strong lyric search w/ selenium + genius api
</commit_message>
<xml_diff>
--- a/exports/Top 100.xlsx
+++ b/exports/Top 100.xlsx
@@ -1509,7 +1509,7 @@
         <v>0.1423076923076923</v>
       </c>
       <c r="Q2">
-        <v>0.3676923076923078</v>
+        <v>0.3676923076923077</v>
       </c>
       <c r="R2">
         <v>0.6861538461538461</v>
@@ -1630,7 +1630,7 @@
         <v>0.2745454545454546</v>
       </c>
       <c r="P4">
-        <v>0.05545454545454546</v>
+        <v>0.05545454545454545</v>
       </c>
       <c r="Q4">
         <v>0.2090909090909091</v>
@@ -1689,7 +1689,7 @@
         <v>0.207391304347826</v>
       </c>
       <c r="O5">
-        <v>0.31</v>
+        <v>0.3100000000000001</v>
       </c>
       <c r="P5">
         <v>0.0456521739130435</v>
@@ -1748,10 +1748,10 @@
         <v>212</v>
       </c>
       <c r="N6">
-        <v>0.7185294117647061</v>
+        <v>0.718529411764706</v>
       </c>
       <c r="O6">
-        <v>0.5014705882352941</v>
+        <v>0.5014705882352942</v>
       </c>
       <c r="P6">
         <v>0.1923529411764706</v>
@@ -1760,7 +1760,7 @@
         <v>0.4447058823529412</v>
       </c>
       <c r="R6">
-        <v>0.3970588235294117</v>
+        <v>0.3970588235294118</v>
       </c>
       <c r="S6">
         <v>0.2102941176470589</v>
@@ -1946,7 +1946,7 @@
         <v>0.215</v>
       </c>
       <c r="R9">
-        <v>0.6633333333333333</v>
+        <v>0.6633333333333334</v>
       </c>
       <c r="S9">
         <v>0.17</v>
@@ -1999,7 +1999,7 @@
         <v>0.1235714285714286</v>
       </c>
       <c r="O10">
-        <v>0.5921428571428571</v>
+        <v>0.5921428571428572</v>
       </c>
       <c r="P10">
         <v>0.2921428571428571</v>
@@ -2008,7 +2008,7 @@
         <v>0.3114285714285714</v>
       </c>
       <c r="R10">
-        <v>0.6657142857142857</v>
+        <v>0.6657142857142858</v>
       </c>
       <c r="S10">
         <v>0.3307142857142857</v>
@@ -2055,13 +2055,13 @@
         <v>335</v>
       </c>
       <c r="M11">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N11">
         <v>0.7677777777777778</v>
       </c>
       <c r="O11">
-        <v>0.5622222222222222</v>
+        <v>0.5622222222222223</v>
       </c>
       <c r="P11">
         <v>0.05222222222222222</v>
@@ -2132,10 +2132,10 @@
         <v>0.09999999999999999</v>
       </c>
       <c r="R12">
-        <v>0.6185714285714285</v>
+        <v>0.6185714285714287</v>
       </c>
       <c r="S12">
-        <v>0.1871428571428571</v>
+        <v>0.1871428571428572</v>
       </c>
       <c r="T12">
         <v>0.89</v>
@@ -2241,7 +2241,7 @@
         <v>336</v>
       </c>
       <c r="M14">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="N14">
         <v>0.1057142857142857</v>
@@ -2250,13 +2250,13 @@
         <v>0.3835714285714286</v>
       </c>
       <c r="P14">
-        <v>0.08</v>
+        <v>0.07999999999999999</v>
       </c>
       <c r="Q14">
         <v>0.36</v>
       </c>
       <c r="R14">
-        <v>0.8014285714285715</v>
+        <v>0.8014285714285713</v>
       </c>
       <c r="S14">
         <v>0.2064285714285714</v>
@@ -2312,7 +2312,7 @@
         <v>0.3235</v>
       </c>
       <c r="P15">
-        <v>0.05950000000000001</v>
+        <v>0.05950000000000002</v>
       </c>
       <c r="Q15">
         <v>0.191</v>
@@ -2324,7 +2324,7 @@
         <v>0.1425</v>
       </c>
       <c r="T15">
-        <v>0.6015</v>
+        <v>0.6014999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -2365,7 +2365,7 @@
         <v>336</v>
       </c>
       <c r="M16">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N16">
         <v>0.945</v>
@@ -2433,16 +2433,16 @@
         <v>0.3846666666666667</v>
       </c>
       <c r="O17">
-        <v>0.5946666666666666</v>
+        <v>0.5946666666666667</v>
       </c>
       <c r="P17">
         <v>0.1546666666666667</v>
       </c>
       <c r="Q17">
-        <v>0.5473333333333333</v>
+        <v>0.5473333333333332</v>
       </c>
       <c r="R17">
-        <v>0.6039999999999999</v>
+        <v>0.604</v>
       </c>
       <c r="S17">
         <v>0.3526666666666667</v>
@@ -2492,7 +2492,7 @@
         <v>33</v>
       </c>
       <c r="N18">
-        <v>0.8736363636363635</v>
+        <v>0.8736363636363634</v>
       </c>
       <c r="O18">
         <v>0.6145454545454546</v>
@@ -2501,7 +2501,7 @@
         <v>0.04272727272727272</v>
       </c>
       <c r="Q18">
-        <v>0.5027272727272727</v>
+        <v>0.5027272727272728</v>
       </c>
       <c r="R18">
         <v>0.3190909090909091</v>
@@ -2560,10 +2560,10 @@
         <v>0.6869230769230769</v>
       </c>
       <c r="P19">
-        <v>0.04384615384615383</v>
+        <v>0.04384615384615385</v>
       </c>
       <c r="Q19">
-        <v>0.4876923076923077</v>
+        <v>0.4876923076923078</v>
       </c>
       <c r="R19">
         <v>0.5861538461538461</v>
@@ -2613,7 +2613,7 @@
         <v>336</v>
       </c>
       <c r="M20">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N20">
         <v>0.945</v>
@@ -2752,13 +2752,13 @@
         <v>0.4392307692307693</v>
       </c>
       <c r="R22">
-        <v>0.8461538461538463</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="S22">
         <v>0.1876923076923077</v>
       </c>
       <c r="T22">
-        <v>0.2553846153846153</v>
+        <v>0.2553846153846154</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -2867,13 +2867,13 @@
         <v>0.008666666666666666</v>
       </c>
       <c r="O24">
-        <v>0.5866666666666666</v>
+        <v>0.5866666666666667</v>
       </c>
       <c r="P24">
         <v>0.04600000000000001</v>
       </c>
       <c r="Q24">
-        <v>0.6133333333333333</v>
+        <v>0.6133333333333332</v>
       </c>
       <c r="R24">
         <v>0.6093333333333334</v>
@@ -2991,7 +2991,7 @@
         <v>0.189</v>
       </c>
       <c r="O26">
-        <v>0.4029999999999999</v>
+        <v>0.403</v>
       </c>
       <c r="P26">
         <v>0.036</v>
@@ -3118,16 +3118,16 @@
         <v>0.6738461538461539</v>
       </c>
       <c r="P28">
-        <v>0.1776923076923076</v>
+        <v>0.1776923076923077</v>
       </c>
       <c r="Q28">
-        <v>0.4015384615384615</v>
+        <v>0.4015384615384616</v>
       </c>
       <c r="R28">
-        <v>0.6653846153846152</v>
+        <v>0.6653846153846155</v>
       </c>
       <c r="S28">
-        <v>0.2269230769230769</v>
+        <v>0.226923076923077</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -3248,7 +3248,7 @@
         <v>0.2735714285714286</v>
       </c>
       <c r="R30">
-        <v>0.4485714285714286</v>
+        <v>0.4485714285714285</v>
       </c>
       <c r="S30">
         <v>0.1392857142857143</v>
@@ -3310,7 +3310,7 @@
         <v>0.3391666666666667</v>
       </c>
       <c r="R31">
-        <v>0.5966666666666667</v>
+        <v>0.5966666666666666</v>
       </c>
       <c r="S31">
         <v>0.2291666666666667</v>
@@ -3546,7 +3546,7 @@
         <v>0.4873333333333333</v>
       </c>
       <c r="R35">
-        <v>0.712</v>
+        <v>0.7120000000000001</v>
       </c>
       <c r="S35">
         <v>0.3286666666666667</v>
@@ -3593,7 +3593,7 @@
         <v>15</v>
       </c>
       <c r="N36">
-        <v>0.421875</v>
+        <v>0.4218749999999999</v>
       </c>
       <c r="O36">
         <v>0.555</v>
@@ -3602,7 +3602,7 @@
         <v>0.135</v>
       </c>
       <c r="Q36">
-        <v>0.4012499999999999</v>
+        <v>0.4012500000000001</v>
       </c>
       <c r="R36">
         <v>0.4637499999999999</v>
@@ -3652,7 +3652,7 @@
         <v>81</v>
       </c>
       <c r="N37">
-        <v>0.4318750000000001</v>
+        <v>0.431875</v>
       </c>
       <c r="O37">
         <v>0.54125</v>
@@ -3661,16 +3661,16 @@
         <v>0.04125</v>
       </c>
       <c r="Q37">
-        <v>0.359375</v>
+        <v>0.3593750000000001</v>
       </c>
       <c r="R37">
-        <v>0.6031249999999999</v>
+        <v>0.603125</v>
       </c>
       <c r="S37">
         <v>0.1725</v>
       </c>
       <c r="T37">
-        <v>0.46625</v>
+        <v>0.4662500000000001</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -3720,7 +3720,7 @@
         <v>0.09181818181818181</v>
       </c>
       <c r="Q38">
-        <v>0.4081818181818182</v>
+        <v>0.4081818181818181</v>
       </c>
       <c r="R38">
         <v>0.8236363636363637</v>
@@ -3770,7 +3770,7 @@
         <v>51</v>
       </c>
       <c r="N39">
-        <v>0.3642857142857143</v>
+        <v>0.3642857142857142</v>
       </c>
       <c r="O39">
         <v>0.5785714285714286</v>
@@ -3782,7 +3782,7 @@
         <v>0.6557142857142857</v>
       </c>
       <c r="R39">
-        <v>0.5952380952380951</v>
+        <v>0.5952380952380952</v>
       </c>
       <c r="S39">
         <v>0.3371428571428571</v>
@@ -3835,7 +3835,7 @@
         <v>0.3317857142857142</v>
       </c>
       <c r="P40">
-        <v>0.03857142857142859</v>
+        <v>0.03857142857142858</v>
       </c>
       <c r="Q40">
         <v>0.36</v>
@@ -3888,7 +3888,7 @@
         <v>68</v>
       </c>
       <c r="N41">
-        <v>0.07916666666666666</v>
+        <v>0.07916666666666668</v>
       </c>
       <c r="O41">
         <v>0.4216666666666667</v>
@@ -4121,7 +4121,7 @@
         <v>338</v>
       </c>
       <c r="M45">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="N45">
         <v>0.3684615384615384</v>
@@ -4186,7 +4186,7 @@
         <v>0.2809090909090909</v>
       </c>
       <c r="O46">
-        <v>0.5345454545454547</v>
+        <v>0.5345454545454545</v>
       </c>
       <c r="P46">
         <v>0.03000000000000001</v>
@@ -4251,7 +4251,7 @@
         <v>0.03545454545454545</v>
       </c>
       <c r="Q47">
-        <v>0.6927272727272729</v>
+        <v>0.6927272727272727</v>
       </c>
       <c r="R47">
         <v>0.7836363636363636</v>
@@ -4260,7 +4260,7 @@
         <v>0.1645454545454546</v>
       </c>
       <c r="T47">
-        <v>0.2654545454545455</v>
+        <v>0.2654545454545454</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -4307,13 +4307,13 @@
         <v>0.3458333333333334</v>
       </c>
       <c r="P48">
-        <v>0.08916666666666666</v>
+        <v>0.08916666666666667</v>
       </c>
       <c r="Q48">
         <v>0.3008333333333333</v>
       </c>
       <c r="R48">
-        <v>0.8775000000000001</v>
+        <v>0.8774999999999999</v>
       </c>
       <c r="S48">
         <v>0.1566666666666667</v>
@@ -4549,7 +4549,7 @@
         <v>0.16875</v>
       </c>
       <c r="R52">
-        <v>0.9224999999999999</v>
+        <v>0.9225000000000001</v>
       </c>
       <c r="S52">
         <v>0.1875</v>
@@ -4593,7 +4593,7 @@
         <v>339</v>
       </c>
       <c r="M53">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N53">
         <v>0.1657142857142857</v>
@@ -4605,10 +4605,10 @@
         <v>0.08785714285714287</v>
       </c>
       <c r="Q53">
-        <v>0.4392857142857143</v>
+        <v>0.4392857142857142</v>
       </c>
       <c r="R53">
-        <v>0.6178571428571428</v>
+        <v>0.6178571428571429</v>
       </c>
       <c r="S53">
         <v>0.1878571428571429</v>
@@ -4726,7 +4726,7 @@
         <v>0.4858333333333333</v>
       </c>
       <c r="R55">
-        <v>0.5666666666666668</v>
+        <v>0.5666666666666665</v>
       </c>
       <c r="S55">
         <v>0.2341666666666667</v>
@@ -4785,7 +4785,7 @@
         <v>0.1466666666666666</v>
       </c>
       <c r="R56">
-        <v>0.5191666666666667</v>
+        <v>0.5191666666666668</v>
       </c>
       <c r="S56">
         <v>0.1333333333333333</v>
@@ -4891,25 +4891,25 @@
         <v>8</v>
       </c>
       <c r="N58">
-        <v>0.03333333333333334</v>
+        <v>0.1569230769230769</v>
       </c>
       <c r="O58">
-        <v>0.4233333333333333</v>
+        <v>0.4415384615384616</v>
       </c>
       <c r="P58">
-        <v>0.04777777777777778</v>
+        <v>0.04538461538461538</v>
       </c>
       <c r="Q58">
-        <v>0.1533333333333333</v>
+        <v>0.1484615384615385</v>
       </c>
       <c r="R58">
-        <v>0.7255555555555556</v>
+        <v>0.6538461538461539</v>
       </c>
       <c r="S58">
-        <v>0.1644444444444445</v>
+        <v>0.1453846153846154</v>
       </c>
       <c r="T58">
-        <v>0.27</v>
+        <v>0.2423076923076923</v>
       </c>
     </row>
     <row r="59" spans="1:20">
@@ -5077,7 +5077,7 @@
         <v>0.05928571428571429</v>
       </c>
       <c r="Q61">
-        <v>0.5785714285714286</v>
+        <v>0.5785714285714285</v>
       </c>
       <c r="R61">
         <v>0.8757142857142857</v>
@@ -5183,13 +5183,13 @@
         <v>339</v>
       </c>
       <c r="M63">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="N63">
         <v>0.01333333333333333</v>
       </c>
       <c r="O63">
-        <v>0.3658333333333334</v>
+        <v>0.3658333333333332</v>
       </c>
       <c r="P63">
         <v>0.09833333333333333</v>
@@ -5496,7 +5496,7 @@
         <v>0.6590909090909091</v>
       </c>
       <c r="S68">
-        <v>0.1745454545454545</v>
+        <v>0.1745454545454546</v>
       </c>
       <c r="T68">
         <v>0.7663636363636364</v>
@@ -5658,19 +5658,19 @@
         <v>16</v>
       </c>
       <c r="N71">
-        <v>0.6621428571428573</v>
+        <v>0.6621428571428571</v>
       </c>
       <c r="O71">
         <v>0.4814285714285714</v>
       </c>
       <c r="P71">
-        <v>0.04357142857142858</v>
+        <v>0.04357142857142857</v>
       </c>
       <c r="Q71">
         <v>0.205</v>
       </c>
       <c r="R71">
-        <v>0.3842857142857143</v>
+        <v>0.3842857142857142</v>
       </c>
       <c r="S71">
         <v>0.1278571428571429</v>
@@ -5723,13 +5723,13 @@
         <v>0.46875</v>
       </c>
       <c r="P72">
-        <v>0.04875000000000001</v>
+        <v>0.04875000000000002</v>
       </c>
       <c r="Q72">
         <v>0.405</v>
       </c>
       <c r="R72">
-        <v>0.720625</v>
+        <v>0.7206249999999998</v>
       </c>
       <c r="S72">
         <v>0.20625</v>

</xml_diff>

<commit_message>
files cleaned, all helpers integrated to BaseClasses
</commit_message>
<xml_diff>
--- a/exports/Top 100.xlsx
+++ b/exports/Top 100.xlsx
@@ -1509,7 +1509,7 @@
         <v>0.1423076923076923</v>
       </c>
       <c r="Q2">
-        <v>0.3676923076923077</v>
+        <v>0.3676923076923078</v>
       </c>
       <c r="R2">
         <v>0.6861538461538461</v>
@@ -1630,7 +1630,7 @@
         <v>0.2745454545454546</v>
       </c>
       <c r="P4">
-        <v>0.05545454545454545</v>
+        <v>0.05545454545454546</v>
       </c>
       <c r="Q4">
         <v>0.2090909090909091</v>
@@ -1686,13 +1686,13 @@
         <v>25</v>
       </c>
       <c r="N5">
-        <v>0.207391304347826</v>
+        <v>0.2073913043478261</v>
       </c>
       <c r="O5">
         <v>0.31</v>
       </c>
       <c r="P5">
-        <v>0.0456521739130435</v>
+        <v>0.04565217391304349</v>
       </c>
       <c r="Q5">
         <v>0.2530434782608696</v>
@@ -1745,7 +1745,7 @@
         <v>334</v>
       </c>
       <c r="M6">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="N6">
         <v>0.7185294117647061</v>
@@ -1810,10 +1810,10 @@
         <v>3</v>
       </c>
       <c r="N7">
-        <v>0.2241666666666667</v>
+        <v>0.2241666666666666</v>
       </c>
       <c r="O7">
-        <v>0.405</v>
+        <v>0.4050000000000001</v>
       </c>
       <c r="P7">
         <v>0.1075</v>
@@ -1869,13 +1869,13 @@
         <v>335</v>
       </c>
       <c r="M8">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N8">
         <v>0.1725</v>
       </c>
       <c r="O8">
-        <v>0.4399999999999999</v>
+        <v>0.44</v>
       </c>
       <c r="P8">
         <v>0.04916666666666667</v>
@@ -1993,7 +1993,7 @@
         <v>335</v>
       </c>
       <c r="M10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N10">
         <v>0.1235714285714286</v>
@@ -2064,7 +2064,7 @@
         <v>0.5622222222222223</v>
       </c>
       <c r="P11">
-        <v>0.05222222222222221</v>
+        <v>0.05222222222222222</v>
       </c>
       <c r="Q11">
         <v>0.2977777777777778</v>
@@ -2185,10 +2185,10 @@
         <v>0.4758333333333333</v>
       </c>
       <c r="O13">
-        <v>0.41</v>
+        <v>0.4100000000000001</v>
       </c>
       <c r="P13">
-        <v>0.03333333333333333</v>
+        <v>0.03333333333333335</v>
       </c>
       <c r="Q13">
         <v>0.3425</v>
@@ -2256,10 +2256,10 @@
         <v>0.36</v>
       </c>
       <c r="R14">
-        <v>0.8014285714285714</v>
+        <v>0.8014285714285715</v>
       </c>
       <c r="S14">
-        <v>0.2064285714285715</v>
+        <v>0.2064285714285714</v>
       </c>
       <c r="T14">
         <v>0.001428571428571429</v>
@@ -2312,7 +2312,7 @@
         <v>0.3235</v>
       </c>
       <c r="P15">
-        <v>0.05950000000000001</v>
+        <v>0.05950000000000002</v>
       </c>
       <c r="Q15">
         <v>0.191</v>
@@ -2433,7 +2433,7 @@
         <v>0.3846666666666667</v>
       </c>
       <c r="O17">
-        <v>0.5946666666666667</v>
+        <v>0.5946666666666666</v>
       </c>
       <c r="P17">
         <v>0.1546666666666667</v>
@@ -2566,7 +2566,7 @@
         <v>0.4876923076923077</v>
       </c>
       <c r="R19">
-        <v>0.5861538461538462</v>
+        <v>0.5861538461538461</v>
       </c>
       <c r="S19">
         <v>0.1330769230769231</v>
@@ -2746,19 +2746,19 @@
         <v>0.4615384615384616</v>
       </c>
       <c r="P22">
-        <v>0.09538461538461539</v>
+        <v>0.0953846153846154</v>
       </c>
       <c r="Q22">
-        <v>0.4392307692307693</v>
+        <v>0.4392307692307692</v>
       </c>
       <c r="R22">
-        <v>0.8461538461538463</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="S22">
         <v>0.1876923076923077</v>
       </c>
       <c r="T22">
-        <v>0.2553846153846153</v>
+        <v>0.2553846153846154</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -2861,7 +2861,7 @@
         <v>336</v>
       </c>
       <c r="M24">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="N24">
         <v>0.008666666666666666</v>
@@ -2876,7 +2876,7 @@
         <v>0.6133333333333333</v>
       </c>
       <c r="R24">
-        <v>0.6093333333333335</v>
+        <v>0.6093333333333334</v>
       </c>
       <c r="S24">
         <v>0.132</v>
@@ -2929,13 +2929,13 @@
         <v>0.3545454545454544</v>
       </c>
       <c r="O25">
-        <v>0.4540909090909091</v>
+        <v>0.4540909090909092</v>
       </c>
       <c r="P25">
-        <v>0.0531818181818182</v>
+        <v>0.05318181818181819</v>
       </c>
       <c r="Q25">
-        <v>0.4390909090909091</v>
+        <v>0.4390909090909092</v>
       </c>
       <c r="R25">
         <v>0.6004545454545456</v>
@@ -2994,13 +2994,13 @@
         <v>0.403</v>
       </c>
       <c r="P26">
-        <v>0.036</v>
+        <v>0.03599999999999999</v>
       </c>
       <c r="Q26">
         <v>0.468</v>
       </c>
       <c r="R26">
-        <v>0.7500000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="S26">
         <v>0.215</v>
@@ -3118,13 +3118,13 @@
         <v>0.6738461538461539</v>
       </c>
       <c r="P28">
-        <v>0.1776923076923076</v>
+        <v>0.1776923076923077</v>
       </c>
       <c r="Q28">
-        <v>0.4015384615384615</v>
+        <v>0.4015384615384616</v>
       </c>
       <c r="R28">
-        <v>0.6653846153846152</v>
+        <v>0.6653846153846155</v>
       </c>
       <c r="S28">
         <v>0.226923076923077</v>
@@ -3177,10 +3177,10 @@
         <v>0.4376666666666666</v>
       </c>
       <c r="O29">
-        <v>0.5433333333333332</v>
+        <v>0.5433333333333333</v>
       </c>
       <c r="P29">
-        <v>0.07433333333333335</v>
+        <v>0.07433333333333336</v>
       </c>
       <c r="Q29">
         <v>0.2736666666666667</v>
@@ -3248,7 +3248,7 @@
         <v>0.2735714285714286</v>
       </c>
       <c r="R30">
-        <v>0.4485714285714285</v>
+        <v>0.4485714285714286</v>
       </c>
       <c r="S30">
         <v>0.1392857142857143</v>
@@ -3307,10 +3307,10 @@
         <v>0.05166666666666667</v>
       </c>
       <c r="Q31">
-        <v>0.3391666666666667</v>
+        <v>0.3391666666666666</v>
       </c>
       <c r="R31">
-        <v>0.5966666666666668</v>
+        <v>0.5966666666666667</v>
       </c>
       <c r="S31">
         <v>0.2291666666666666</v>
@@ -3366,13 +3366,13 @@
         <v>0.1152941176470588</v>
       </c>
       <c r="Q32">
-        <v>0.4900000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="R32">
-        <v>0.8088235294117647</v>
+        <v>0.8088235294117645</v>
       </c>
       <c r="S32">
-        <v>0.1870588235294118</v>
+        <v>0.1870588235294117</v>
       </c>
       <c r="T32">
         <v>0.1252941176470588</v>
@@ -3428,7 +3428,7 @@
         <v>0.1627272727272727</v>
       </c>
       <c r="R33">
-        <v>0.4745454545454545</v>
+        <v>0.4745454545454546</v>
       </c>
       <c r="S33">
         <v>0.2609090909090909</v>
@@ -3472,7 +3472,7 @@
         <v>338</v>
       </c>
       <c r="M34">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N34">
         <v>0.1630769230769231</v>
@@ -3481,13 +3481,13 @@
         <v>0.5023076923076922</v>
       </c>
       <c r="P34">
-        <v>0.05692307692307692</v>
+        <v>0.05692307692307694</v>
       </c>
       <c r="Q34">
         <v>0.4846153846153846</v>
       </c>
       <c r="R34">
-        <v>0.7061538461538462</v>
+        <v>0.7061538461538461</v>
       </c>
       <c r="S34">
         <v>0.1623076923076923</v>
@@ -3537,7 +3537,7 @@
         <v>0.344</v>
       </c>
       <c r="O35">
-        <v>0.5713333333333334</v>
+        <v>0.5713333333333332</v>
       </c>
       <c r="P35">
         <v>0.306</v>
@@ -3590,10 +3590,10 @@
         <v>338</v>
       </c>
       <c r="M36">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="N36">
-        <v>0.421875</v>
+        <v>0.4218749999999999</v>
       </c>
       <c r="O36">
         <v>0.555</v>
@@ -3602,7 +3602,7 @@
         <v>0.135</v>
       </c>
       <c r="Q36">
-        <v>0.40125</v>
+        <v>0.4012500000000001</v>
       </c>
       <c r="R36">
         <v>0.4637499999999999</v>
@@ -3652,7 +3652,7 @@
         <v>81</v>
       </c>
       <c r="N37">
-        <v>0.431875</v>
+        <v>0.4318750000000001</v>
       </c>
       <c r="O37">
         <v>0.54125</v>
@@ -3661,7 +3661,7 @@
         <v>0.04125</v>
       </c>
       <c r="Q37">
-        <v>0.359375</v>
+        <v>0.3593750000000001</v>
       </c>
       <c r="R37">
         <v>0.6031249999999999</v>
@@ -3720,10 +3720,10 @@
         <v>0.09181818181818181</v>
       </c>
       <c r="Q38">
-        <v>0.4081818181818183</v>
+        <v>0.4081818181818182</v>
       </c>
       <c r="R38">
-        <v>0.8236363636363638</v>
+        <v>0.8236363636363637</v>
       </c>
       <c r="S38">
         <v>0.34</v>
@@ -3776,13 +3776,13 @@
         <v>0.5785714285714286</v>
       </c>
       <c r="P39">
-        <v>0.4185714285714284</v>
+        <v>0.4185714285714285</v>
       </c>
       <c r="Q39">
         <v>0.6557142857142857</v>
       </c>
       <c r="R39">
-        <v>0.5952380952380951</v>
+        <v>0.5952380952380952</v>
       </c>
       <c r="S39">
         <v>0.3371428571428571</v>
@@ -3835,7 +3835,7 @@
         <v>0.3317857142857142</v>
       </c>
       <c r="P40">
-        <v>0.03857142857142858</v>
+        <v>0.03857142857142859</v>
       </c>
       <c r="Q40">
         <v>0.36</v>
@@ -3888,7 +3888,7 @@
         <v>68</v>
       </c>
       <c r="N41">
-        <v>0.07916666666666666</v>
+        <v>0.07916666666666668</v>
       </c>
       <c r="O41">
         <v>0.4216666666666667</v>
@@ -3959,7 +3959,7 @@
         <v>0.415</v>
       </c>
       <c r="R42">
-        <v>0.9662499999999999</v>
+        <v>0.9662500000000001</v>
       </c>
       <c r="S42">
         <v>0.2525</v>
@@ -4006,7 +4006,7 @@
         <v>15</v>
       </c>
       <c r="N43">
-        <v>0.2845454545454546</v>
+        <v>0.2845454545454545</v>
       </c>
       <c r="O43">
         <v>0.6463636363636364</v>
@@ -4071,7 +4071,7 @@
         <v>0.371</v>
       </c>
       <c r="P44">
-        <v>0.033</v>
+        <v>0.03300000000000001</v>
       </c>
       <c r="Q44">
         <v>0.2919999999999999</v>
@@ -4133,10 +4133,10 @@
         <v>0.04076923076923077</v>
       </c>
       <c r="Q45">
-        <v>0.1638461538461538</v>
+        <v>0.1638461538461539</v>
       </c>
       <c r="R45">
-        <v>0.4584615384615384</v>
+        <v>0.4584615384615385</v>
       </c>
       <c r="S45">
         <v>0.3176923076923077</v>
@@ -4180,7 +4180,7 @@
         <v>338</v>
       </c>
       <c r="M46">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="N46">
         <v>0.2809090909090909</v>
@@ -4239,7 +4239,7 @@
         <v>338</v>
       </c>
       <c r="M47">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N47">
         <v>0.03272727272727273</v>
@@ -4251,10 +4251,10 @@
         <v>0.03545454545454545</v>
       </c>
       <c r="Q47">
-        <v>0.6927272727272729</v>
+        <v>0.6927272727272727</v>
       </c>
       <c r="R47">
-        <v>0.7836363636363637</v>
+        <v>0.7836363636363636</v>
       </c>
       <c r="S47">
         <v>0.1645454545454546</v>
@@ -4316,7 +4316,7 @@
         <v>0.8775000000000001</v>
       </c>
       <c r="S48">
-        <v>0.1566666666666666</v>
+        <v>0.1566666666666667</v>
       </c>
       <c r="T48">
         <v>0.1525</v>
@@ -4363,13 +4363,13 @@
         <v>0.24</v>
       </c>
       <c r="O49">
-        <v>0.5141666666666668</v>
+        <v>0.5141666666666667</v>
       </c>
       <c r="P49">
         <v>0.04250000000000001</v>
       </c>
       <c r="Q49">
-        <v>0.4125</v>
+        <v>0.4125000000000001</v>
       </c>
       <c r="R49">
         <v>0.7316666666666665</v>
@@ -4425,7 +4425,7 @@
         <v>0.42125</v>
       </c>
       <c r="P50">
-        <v>0.06749999999999999</v>
+        <v>0.0675</v>
       </c>
       <c r="Q50">
         <v>0.4225</v>
@@ -4437,7 +4437,7 @@
         <v>0.1425</v>
       </c>
       <c r="T50">
-        <v>0.5075</v>
+        <v>0.5075000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -4487,7 +4487,7 @@
         <v>0.09411764705882354</v>
       </c>
       <c r="Q51">
-        <v>0.3176470588235294</v>
+        <v>0.3176470588235295</v>
       </c>
       <c r="R51">
         <v>0.6388235294117649</v>
@@ -4549,7 +4549,7 @@
         <v>0.16875</v>
       </c>
       <c r="R52">
-        <v>0.9224999999999999</v>
+        <v>0.9225</v>
       </c>
       <c r="S52">
         <v>0.1875</v>
@@ -4593,16 +4593,16 @@
         <v>339</v>
       </c>
       <c r="M53">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="N53">
         <v>0.1657142857142857</v>
       </c>
       <c r="O53">
-        <v>0.667142857142857</v>
+        <v>0.6671428571428571</v>
       </c>
       <c r="P53">
-        <v>0.08785714285714287</v>
+        <v>0.08785714285714286</v>
       </c>
       <c r="Q53">
         <v>0.4392857142857142</v>
@@ -4726,7 +4726,7 @@
         <v>0.4858333333333333</v>
       </c>
       <c r="R55">
-        <v>0.5666666666666665</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="S55">
         <v>0.2341666666666667</v>
@@ -4770,7 +4770,7 @@
         <v>339</v>
       </c>
       <c r="M56">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="N56">
         <v>0.4383333333333334</v>
@@ -4888,28 +4888,28 @@
         <v>339</v>
       </c>
       <c r="M58">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N58">
-        <v>0.1569230769230769</v>
+        <v>0.03333333333333334</v>
       </c>
       <c r="O58">
-        <v>0.4415384615384615</v>
+        <v>0.4233333333333333</v>
       </c>
       <c r="P58">
-        <v>0.04538461538461539</v>
+        <v>0.04777777777777778</v>
       </c>
       <c r="Q58">
-        <v>0.1484615384615385</v>
+        <v>0.1533333333333333</v>
       </c>
       <c r="R58">
-        <v>0.653846153846154</v>
+        <v>0.7255555555555556</v>
       </c>
       <c r="S58">
-        <v>0.1453846153846154</v>
+        <v>0.1644444444444445</v>
       </c>
       <c r="T58">
-        <v>0.2423076923076923</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="59" spans="1:20">
@@ -4947,13 +4947,13 @@
         <v>339</v>
       </c>
       <c r="M59">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N59">
         <v>0.075</v>
       </c>
       <c r="O59">
-        <v>0.4991666666666666</v>
+        <v>0.4991666666666667</v>
       </c>
       <c r="P59">
         <v>0.06833333333333334</v>
@@ -4962,7 +4962,7 @@
         <v>0.5658333333333333</v>
       </c>
       <c r="R59">
-        <v>0.8275</v>
+        <v>0.8275000000000001</v>
       </c>
       <c r="S59">
         <v>0.1358333333333333</v>
@@ -5068,19 +5068,19 @@
         <v>18</v>
       </c>
       <c r="N61">
-        <v>0.07428571428571429</v>
+        <v>0.0742857142857143</v>
       </c>
       <c r="O61">
-        <v>0.5735714285714285</v>
+        <v>0.5735714285714286</v>
       </c>
       <c r="P61">
-        <v>0.05928571428571431</v>
+        <v>0.05928571428571429</v>
       </c>
       <c r="Q61">
-        <v>0.5785714285714285</v>
+        <v>0.5785714285714286</v>
       </c>
       <c r="R61">
-        <v>0.8757142857142856</v>
+        <v>0.8757142857142857</v>
       </c>
       <c r="S61">
         <v>0.1835714285714286</v>
@@ -5183,7 +5183,7 @@
         <v>339</v>
       </c>
       <c r="M63">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="N63">
         <v>0.01333333333333333</v>
@@ -5192,7 +5192,7 @@
         <v>0.3658333333333334</v>
       </c>
       <c r="P63">
-        <v>0.09833333333333334</v>
+        <v>0.09833333333333333</v>
       </c>
       <c r="Q63">
         <v>0.2633333333333334</v>
@@ -5254,7 +5254,7 @@
         <v>0.1030769230769231</v>
       </c>
       <c r="Q64">
-        <v>0.4407692307692307</v>
+        <v>0.4407692307692308</v>
       </c>
       <c r="R64">
         <v>0.5207692307692308</v>
@@ -5487,7 +5487,7 @@
         <v>0.3718181818181818</v>
       </c>
       <c r="P68">
-        <v>0.03272727272727273</v>
+        <v>0.03272727272727272</v>
       </c>
       <c r="Q68">
         <v>0.2463636363636364</v>
@@ -5543,13 +5543,13 @@
         <v>0.271</v>
       </c>
       <c r="O69">
-        <v>0.6540000000000001</v>
+        <v>0.654</v>
       </c>
       <c r="P69">
         <v>0.095</v>
       </c>
       <c r="Q69">
-        <v>0.5700000000000001</v>
+        <v>0.57</v>
       </c>
       <c r="R69">
         <v>0.548</v>
@@ -5676,7 +5676,7 @@
         <v>0.1278571428571429</v>
       </c>
       <c r="T71">
-        <v>0.2421428571428571</v>
+        <v>0.2421428571428572</v>
       </c>
     </row>
     <row r="72" spans="1:20">
@@ -5720,13 +5720,13 @@
         <v>0.2175</v>
       </c>
       <c r="O72">
-        <v>0.46875</v>
+        <v>0.4687499999999999</v>
       </c>
       <c r="P72">
-        <v>0.04875000000000002</v>
+        <v>0.04875000000000001</v>
       </c>
       <c r="Q72">
-        <v>0.4050000000000001</v>
+        <v>0.405</v>
       </c>
       <c r="R72">
         <v>0.720625</v>
@@ -5782,13 +5782,13 @@
         <v>0.5021052631578948</v>
       </c>
       <c r="P73">
-        <v>0.04684210526315791</v>
+        <v>0.0468421052631579</v>
       </c>
       <c r="Q73">
         <v>0.4747368421052631</v>
       </c>
       <c r="R73">
-        <v>0.5910526315789473</v>
+        <v>0.5910526315789475</v>
       </c>
       <c r="S73">
         <v>0.2057894736842105</v>

</xml_diff>

<commit_message>
updated secure credential loader
</commit_message>
<xml_diff>
--- a/exports/Top 100.xlsx
+++ b/exports/Top 100.xlsx
@@ -1588,7 +1588,7 @@
         <v>74</v>
       </c>
       <c r="M4">
-        <v>0.4590000000000001</v>
+        <v>0.459</v>
       </c>
       <c r="N4">
         <v>0.53</v>
@@ -1603,7 +1603,7 @@
         <v>0.592</v>
       </c>
       <c r="R4">
-        <v>0.093</v>
+        <v>0.09299999999999999</v>
       </c>
       <c r="S4">
         <v>0.406</v>
@@ -1644,7 +1644,7 @@
         <v>326</v>
       </c>
       <c r="L5">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M5">
         <v>0.2073913043478261</v>
@@ -1662,7 +1662,7 @@
         <v>0.5856521739130435</v>
       </c>
       <c r="R5">
-        <v>0.1760869565217391</v>
+        <v>0.1760869565217392</v>
       </c>
       <c r="S5">
         <v>0.2460869565217391</v>
@@ -1709,7 +1709,7 @@
         <v>0.2433333333333334</v>
       </c>
       <c r="N6">
-        <v>0.4033333333333333</v>
+        <v>0.4033333333333334</v>
       </c>
       <c r="O6">
         <v>0.1041666666666667</v>
@@ -1718,7 +1718,7 @@
         <v>0.3008333333333333</v>
       </c>
       <c r="Q6">
-        <v>0.6791666666666666</v>
+        <v>0.6791666666666667</v>
       </c>
       <c r="R6">
         <v>0.2983333333333333</v>
@@ -1768,7 +1768,7 @@
         <v>0.7185294117647061</v>
       </c>
       <c r="N7">
-        <v>0.5014705882352942</v>
+        <v>0.501470588235294</v>
       </c>
       <c r="O7">
         <v>0.1923529411764706</v>
@@ -1880,7 +1880,7 @@
         <v>326</v>
       </c>
       <c r="L9">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M9">
         <v>0.1235714285714286</v>
@@ -1898,7 +1898,7 @@
         <v>0.6657142857142857</v>
       </c>
       <c r="R9">
-        <v>0.3307142857142858</v>
+        <v>0.3307142857142857</v>
       </c>
       <c r="S9">
         <v>0.0007142857142857143</v>
@@ -1951,7 +1951,7 @@
         <v>0.0953846153846154</v>
       </c>
       <c r="P10">
-        <v>0.4392307692307692</v>
+        <v>0.4392307692307693</v>
       </c>
       <c r="Q10">
         <v>0.8461538461538461</v>
@@ -1960,7 +1960,7 @@
         <v>0.1876923076923077</v>
       </c>
       <c r="S10">
-        <v>0.2553846153846154</v>
+        <v>0.2553846153846153</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -2013,7 +2013,7 @@
         <v>0.215</v>
       </c>
       <c r="Q11">
-        <v>0.6633333333333334</v>
+        <v>0.6633333333333333</v>
       </c>
       <c r="R11">
         <v>0.17</v>
@@ -2072,7 +2072,7 @@
         <v>0.57875</v>
       </c>
       <c r="Q12">
-        <v>0.6787500000000001</v>
+        <v>0.67875</v>
       </c>
       <c r="R12">
         <v>0.2075</v>
@@ -2131,7 +2131,7 @@
         <v>0.3409090909090909</v>
       </c>
       <c r="Q13">
-        <v>0.8409090909090911</v>
+        <v>0.8409090909090909</v>
       </c>
       <c r="R13">
         <v>0.2354545454545455</v>
@@ -2181,10 +2181,10 @@
         <v>0.4758333333333333</v>
       </c>
       <c r="N14">
-        <v>0.4100000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="O14">
-        <v>0.03333333333333334</v>
+        <v>0.03333333333333335</v>
       </c>
       <c r="P14">
         <v>0.3425</v>
@@ -2249,7 +2249,7 @@
         <v>0.3383333333333334</v>
       </c>
       <c r="Q15">
-        <v>0.5508333333333334</v>
+        <v>0.5508333333333333</v>
       </c>
       <c r="R15">
         <v>0.1416666666666667</v>
@@ -2355,13 +2355,13 @@
         <v>53</v>
       </c>
       <c r="M17">
-        <v>0.601</v>
+        <v>0.6009999999999999</v>
       </c>
       <c r="N17">
         <v>0.3235</v>
       </c>
       <c r="O17">
-        <v>0.05950000000000001</v>
+        <v>0.05950000000000002</v>
       </c>
       <c r="P17">
         <v>0.191</v>
@@ -2470,13 +2470,13 @@
         <v>328</v>
       </c>
       <c r="L19">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M19">
         <v>0.5454545454545454</v>
       </c>
       <c r="N19">
-        <v>0.5363636363636363</v>
+        <v>0.5363636363636364</v>
       </c>
       <c r="O19">
         <v>0.03090909090909091</v>
@@ -2485,7 +2485,7 @@
         <v>0.2827272727272728</v>
       </c>
       <c r="Q19">
-        <v>0.4136363636363636</v>
+        <v>0.4136363636363635</v>
       </c>
       <c r="R19">
         <v>0.17</v>
@@ -2606,7 +2606,7 @@
         <v>0.6093333333333334</v>
       </c>
       <c r="R21">
-        <v>0.132</v>
+        <v>0.1320000000000001</v>
       </c>
       <c r="S21">
         <v>0.256</v>
@@ -2653,13 +2653,13 @@
         <v>0.2869230769230769</v>
       </c>
       <c r="N22">
-        <v>0.6869230769230771</v>
+        <v>0.6869230769230769</v>
       </c>
       <c r="O22">
         <v>0.04384615384615385</v>
       </c>
       <c r="P22">
-        <v>0.4876923076923077</v>
+        <v>0.4876923076923078</v>
       </c>
       <c r="Q22">
         <v>0.5861538461538461</v>
@@ -2712,13 +2712,13 @@
         <v>0.8736363636363635</v>
       </c>
       <c r="N23">
-        <v>0.6145454545454545</v>
+        <v>0.6145454545454546</v>
       </c>
       <c r="O23">
         <v>0.04272727272727272</v>
       </c>
       <c r="P23">
-        <v>0.5027272727272728</v>
+        <v>0.5027272727272727</v>
       </c>
       <c r="Q23">
         <v>0.3190909090909091</v>
@@ -2771,7 +2771,7 @@
         <v>0.189</v>
       </c>
       <c r="N24">
-        <v>0.4029999999999999</v>
+        <v>0.403</v>
       </c>
       <c r="O24">
         <v>0.036</v>
@@ -2827,22 +2827,22 @@
         <v>15</v>
       </c>
       <c r="M25">
-        <v>0.3545454545454544</v>
+        <v>0.3545454545454545</v>
       </c>
       <c r="N25">
-        <v>0.454090909090909</v>
+        <v>0.4540909090909091</v>
       </c>
       <c r="O25">
-        <v>0.05318181818181818</v>
+        <v>0.0531818181818182</v>
       </c>
       <c r="P25">
-        <v>0.4390909090909091</v>
+        <v>0.4390909090909092</v>
       </c>
       <c r="Q25">
         <v>0.6004545454545455</v>
       </c>
       <c r="R25">
-        <v>0.8454545454545456</v>
+        <v>0.8454545454545453</v>
       </c>
       <c r="S25">
         <v>0.025</v>
@@ -2889,7 +2889,7 @@
         <v>0.07071428571428572</v>
       </c>
       <c r="N26">
-        <v>0.3317857142857143</v>
+        <v>0.3317857142857142</v>
       </c>
       <c r="O26">
         <v>0.03857142857142859</v>
@@ -2898,7 +2898,7 @@
         <v>0.36</v>
       </c>
       <c r="Q26">
-        <v>0.7957142857142857</v>
+        <v>0.7957142857142859</v>
       </c>
       <c r="R26">
         <v>0.1789285714285714</v>
@@ -2945,7 +2945,7 @@
         <v>48</v>
       </c>
       <c r="M27">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="N27">
         <v>0.3854545454545455</v>
@@ -3007,13 +3007,13 @@
         <v>0.3846666666666667</v>
       </c>
       <c r="N28">
-        <v>0.5946666666666666</v>
+        <v>0.5946666666666667</v>
       </c>
       <c r="O28">
         <v>0.1546666666666666</v>
       </c>
       <c r="P28">
-        <v>0.5473333333333333</v>
+        <v>0.5473333333333332</v>
       </c>
       <c r="Q28">
         <v>0.604</v>
@@ -3060,10 +3060,10 @@
         <v>329</v>
       </c>
       <c r="L29">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M29">
-        <v>0.6399999999999999</v>
+        <v>0.64</v>
       </c>
       <c r="N29">
         <v>0.5285714285714285</v>
@@ -3072,7 +3072,7 @@
         <v>0.06857142857142859</v>
       </c>
       <c r="P29">
-        <v>0.2735714285714286</v>
+        <v>0.2735714285714285</v>
       </c>
       <c r="Q29">
         <v>0.4485714285714285</v>
@@ -3119,7 +3119,7 @@
         <v>329</v>
       </c>
       <c r="L30">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M30">
         <v>0.1316666666666667</v>
@@ -3131,16 +3131,16 @@
         <v>0.05166666666666667</v>
       </c>
       <c r="P30">
-        <v>0.3391666666666667</v>
+        <v>0.3391666666666666</v>
       </c>
       <c r="Q30">
         <v>0.5966666666666668</v>
       </c>
       <c r="R30">
-        <v>0.2291666666666667</v>
+        <v>0.2291666666666666</v>
       </c>
       <c r="S30">
-        <v>0.3</v>
+        <v>0.2999999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -3243,19 +3243,19 @@
         <v>0.4376666666666666</v>
       </c>
       <c r="N32">
-        <v>0.5433333333333333</v>
+        <v>0.5433333333333334</v>
       </c>
       <c r="O32">
-        <v>0.07433333333333335</v>
+        <v>0.07433333333333336</v>
       </c>
       <c r="P32">
-        <v>0.2736666666666666</v>
+        <v>0.2736666666666667</v>
       </c>
       <c r="Q32">
-        <v>0.5813333333333333</v>
+        <v>0.5813333333333335</v>
       </c>
       <c r="R32">
-        <v>0.2473333333333334</v>
+        <v>0.2473333333333333</v>
       </c>
       <c r="S32">
         <v>0.008</v>
@@ -3420,7 +3420,7 @@
         <v>0.2809090909090909</v>
       </c>
       <c r="N35">
-        <v>0.5345454545454545</v>
+        <v>0.5345454545454547</v>
       </c>
       <c r="O35">
         <v>0.03000000000000001</v>
@@ -3479,7 +3479,7 @@
         <v>0.4472727272727273</v>
       </c>
       <c r="N36">
-        <v>0.3754545454545454</v>
+        <v>0.3754545454545455</v>
       </c>
       <c r="O36">
         <v>0.03454545454545455</v>
@@ -3547,7 +3547,7 @@
         <v>0.415</v>
       </c>
       <c r="Q37">
-        <v>0.9662499999999999</v>
+        <v>0.9662500000000001</v>
       </c>
       <c r="R37">
         <v>0.2525</v>
@@ -3591,10 +3591,10 @@
         <v>329</v>
       </c>
       <c r="L38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M38">
-        <v>0.4218749999999999</v>
+        <v>0.4218750000000001</v>
       </c>
       <c r="N38">
         <v>0.555</v>
@@ -3665,7 +3665,7 @@
         <v>0.4081818181818182</v>
       </c>
       <c r="Q39">
-        <v>0.8236363636363637</v>
+        <v>0.8236363636363638</v>
       </c>
       <c r="R39">
         <v>0.34</v>
@@ -3709,7 +3709,7 @@
         <v>329</v>
       </c>
       <c r="L40">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M40">
         <v>0.1630769230769231</v>
@@ -3780,10 +3780,10 @@
         <v>0.03545454545454545</v>
       </c>
       <c r="P41">
-        <v>0.6927272727272727</v>
+        <v>0.6927272727272729</v>
       </c>
       <c r="Q41">
-        <v>0.7836363636363636</v>
+        <v>0.7836363636363637</v>
       </c>
       <c r="R41">
         <v>0.1645454545454546</v>
@@ -3836,10 +3836,10 @@
         <v>0.5141666666666667</v>
       </c>
       <c r="O42">
-        <v>0.0425</v>
+        <v>0.04250000000000001</v>
       </c>
       <c r="P42">
-        <v>0.4125</v>
+        <v>0.4125000000000001</v>
       </c>
       <c r="Q42">
         <v>0.7316666666666665</v>
@@ -3848,7 +3848,7 @@
         <v>0.23</v>
       </c>
       <c r="S42">
-        <v>0.4483333333333333</v>
+        <v>0.4483333333333334</v>
       </c>
     </row>
     <row r="43" spans="1:19">
@@ -3960,7 +3960,7 @@
         <v>0.4873333333333333</v>
       </c>
       <c r="Q44">
-        <v>0.7120000000000001</v>
+        <v>0.7119999999999999</v>
       </c>
       <c r="R44">
         <v>0.3286666666666667</v>
@@ -4078,7 +4078,7 @@
         <v>0.6557142857142857</v>
       </c>
       <c r="Q46">
-        <v>0.5952380952380951</v>
+        <v>0.5952380952380952</v>
       </c>
       <c r="R46">
         <v>0.3371428571428571</v>
@@ -4122,28 +4122,28 @@
         <v>330</v>
       </c>
       <c r="L47">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M47">
-        <v>0.2155</v>
+        <v>0.2033333333333333</v>
       </c>
       <c r="N47">
-        <v>0.2554999999999999</v>
+        <v>0.268</v>
       </c>
       <c r="O47">
-        <v>0.05700000000000001</v>
+        <v>0.05533333333333334</v>
       </c>
       <c r="P47">
-        <v>0.1275</v>
+        <v>0.1366666666666667</v>
       </c>
       <c r="Q47">
-        <v>0.5625</v>
+        <v>0.5533333333333332</v>
       </c>
       <c r="R47">
-        <v>0.146</v>
+        <v>0.16</v>
       </c>
       <c r="S47">
-        <v>0.5534999999999999</v>
+        <v>0.5433333333333332</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -4199,7 +4199,7 @@
         <v>0.8275000000000001</v>
       </c>
       <c r="R48">
-        <v>0.1358333333333333</v>
+        <v>0.1358333333333334</v>
       </c>
       <c r="S48">
         <v>0.009166666666666667</v>
@@ -4358,13 +4358,13 @@
         <v>330</v>
       </c>
       <c r="L51">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M51">
         <v>0.0375</v>
       </c>
       <c r="N51">
-        <v>0.3458333333333334</v>
+        <v>0.3458333333333333</v>
       </c>
       <c r="O51">
         <v>0.08916666666666667</v>
@@ -4373,10 +4373,10 @@
         <v>0.3008333333333333</v>
       </c>
       <c r="Q51">
-        <v>0.8774999999999999</v>
+        <v>0.8775000000000001</v>
       </c>
       <c r="R51">
-        <v>0.1566666666666667</v>
+        <v>0.1566666666666666</v>
       </c>
       <c r="S51">
         <v>0.1525</v>
@@ -4426,7 +4426,7 @@
         <v>0.42125</v>
       </c>
       <c r="O52">
-        <v>0.06749999999999999</v>
+        <v>0.0675</v>
       </c>
       <c r="P52">
         <v>0.4225</v>
@@ -4438,7 +4438,7 @@
         <v>0.1425</v>
       </c>
       <c r="S52">
-        <v>0.5075000000000001</v>
+        <v>0.5075</v>
       </c>
     </row>
     <row r="53" spans="1:19">
@@ -4482,7 +4482,7 @@
         <v>0.1305882352941176</v>
       </c>
       <c r="N53">
-        <v>0.6858823529411765</v>
+        <v>0.6858823529411766</v>
       </c>
       <c r="O53">
         <v>0.09411764705882356</v>
@@ -4541,7 +4541,7 @@
         <v>0.2790740740740741</v>
       </c>
       <c r="N54">
-        <v>0.3838888888888889</v>
+        <v>0.383888888888889</v>
       </c>
       <c r="O54">
         <v>0.03870370370370373</v>
@@ -4553,7 +4553,7 @@
         <v>0.5566666666666666</v>
       </c>
       <c r="R54">
-        <v>0.1844444444444444</v>
+        <v>0.1844444444444443</v>
       </c>
       <c r="S54">
         <v>0.6018518518518519</v>
@@ -4597,13 +4597,13 @@
         <v>20</v>
       </c>
       <c r="M55">
-        <v>0.07428571428571429</v>
+        <v>0.0742857142857143</v>
       </c>
       <c r="N55">
-        <v>0.5735714285714285</v>
+        <v>0.5735714285714286</v>
       </c>
       <c r="O55">
-        <v>0.05928571428571431</v>
+        <v>0.05928571428571429</v>
       </c>
       <c r="P55">
         <v>0.5785714285714285</v>
@@ -4659,13 +4659,13 @@
         <v>0.3953846153846153</v>
       </c>
       <c r="N56">
-        <v>0.51</v>
+        <v>0.5099999999999999</v>
       </c>
       <c r="O56">
         <v>0.1030769230769231</v>
       </c>
       <c r="P56">
-        <v>0.4407692307692307</v>
+        <v>0.4407692307692308</v>
       </c>
       <c r="Q56">
         <v>0.5207692307692308</v>
@@ -4833,7 +4833,7 @@
         <v>90</v>
       </c>
       <c r="M59">
-        <v>0.4318750000000001</v>
+        <v>0.431875</v>
       </c>
       <c r="N59">
         <v>0.54125</v>
@@ -4845,7 +4845,7 @@
         <v>0.3593750000000001</v>
       </c>
       <c r="Q59">
-        <v>0.603125</v>
+        <v>0.6031249999999999</v>
       </c>
       <c r="R59">
         <v>0.1725</v>
@@ -4910,7 +4910,7 @@
         <v>0.1172727272727273</v>
       </c>
       <c r="S60">
-        <v>0.6099999999999999</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="61" spans="1:19">
@@ -4951,25 +4951,25 @@
         <v>7</v>
       </c>
       <c r="M61">
-        <v>0.156923076923077</v>
+        <v>0.03333333333333334</v>
       </c>
       <c r="N61">
-        <v>0.4415384615384616</v>
+        <v>0.4233333333333334</v>
       </c>
       <c r="O61">
-        <v>0.04538461538461538</v>
+        <v>0.04777777777777778</v>
       </c>
       <c r="P61">
-        <v>0.1484615384615385</v>
+        <v>0.1533333333333333</v>
       </c>
       <c r="Q61">
-        <v>0.6538461538461539</v>
+        <v>0.7255555555555555</v>
       </c>
       <c r="R61">
-        <v>0.1453846153846154</v>
+        <v>0.1644444444444445</v>
       </c>
       <c r="S61">
-        <v>0.2423076923076923</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="62" spans="1:19">
@@ -5010,7 +5010,7 @@
         <v>7</v>
       </c>
       <c r="M62">
-        <v>0.4383333333333334</v>
+        <v>0.4383333333333332</v>
       </c>
       <c r="N62">
         <v>0.5575</v>
@@ -5019,13 +5019,13 @@
         <v>0.04333333333333333</v>
       </c>
       <c r="P62">
-        <v>0.1466666666666667</v>
+        <v>0.1466666666666666</v>
       </c>
       <c r="Q62">
-        <v>0.5191666666666667</v>
+        <v>0.5191666666666668</v>
       </c>
       <c r="R62">
-        <v>0.1333333333333334</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="S62">
         <v>0.5525</v>
@@ -5087,7 +5087,7 @@
         <v>0.198</v>
       </c>
       <c r="S63">
-        <v>0.6929999999999998</v>
+        <v>0.6929999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:19">
@@ -5140,7 +5140,7 @@
         <v>0.16875</v>
       </c>
       <c r="Q64">
-        <v>0.9225000000000001</v>
+        <v>0.9225</v>
       </c>
       <c r="R64">
         <v>0.1875</v>
@@ -5187,7 +5187,7 @@
         <v>3</v>
       </c>
       <c r="M65">
-        <v>0.05200000000000001</v>
+        <v>0.052</v>
       </c>
       <c r="N65">
         <v>0.5653333333333332</v>
@@ -5249,19 +5249,19 @@
         <v>0.05</v>
       </c>
       <c r="N66">
-        <v>0.4961538461538462</v>
+        <v>0.4961538461538461</v>
       </c>
       <c r="O66">
-        <v>0.09769230769230769</v>
+        <v>0.09769230769230772</v>
       </c>
       <c r="P66">
         <v>0.4684615384615385</v>
       </c>
       <c r="Q66">
-        <v>0.8761538461538461</v>
+        <v>0.8761538461538462</v>
       </c>
       <c r="R66">
-        <v>0.2507692307692307</v>
+        <v>0.2507692307692308</v>
       </c>
       <c r="S66">
         <v>0.1323076923076923</v>
@@ -5317,10 +5317,10 @@
         <v>0.5738461538461539</v>
       </c>
       <c r="Q67">
-        <v>0.8303846153846154</v>
+        <v>0.8303846153846153</v>
       </c>
       <c r="R67">
-        <v>0.1961538461538462</v>
+        <v>0.1961538461538461</v>
       </c>
       <c r="S67">
         <v>0</v>
@@ -5373,13 +5373,13 @@
         <v>0.2757692307692307</v>
       </c>
       <c r="P68">
-        <v>0.481923076923077</v>
+        <v>0.4819230769230769</v>
       </c>
       <c r="Q68">
-        <v>0.5765384615384614</v>
+        <v>0.5765384615384617</v>
       </c>
       <c r="R68">
-        <v>0.2284615384615384</v>
+        <v>0.2284615384615385</v>
       </c>
       <c r="S68">
         <v>0.006923076923076922</v>
@@ -5435,10 +5435,10 @@
         <v>0.1638461538461538</v>
       </c>
       <c r="Q69">
-        <v>0.4584615384615384</v>
+        <v>0.4584615384615385</v>
       </c>
       <c r="R69">
-        <v>0.3176923076923077</v>
+        <v>0.3176923076923078</v>
       </c>
       <c r="S69">
         <v>0.6900000000000001</v>
@@ -5544,7 +5544,7 @@
         <v>0.2142857142857143</v>
       </c>
       <c r="N71">
-        <v>0.5349999999999999</v>
+        <v>0.535</v>
       </c>
       <c r="O71">
         <v>0.05571428571428572</v>
@@ -5553,7 +5553,7 @@
         <v>0.29</v>
       </c>
       <c r="Q71">
-        <v>0.52</v>
+        <v>0.5200000000000001</v>
       </c>
       <c r="R71">
         <v>0.1814285714285714</v>
@@ -5600,13 +5600,13 @@
         <v>19</v>
       </c>
       <c r="M72">
-        <v>0.6621428571428571</v>
+        <v>0.662142857142857</v>
       </c>
       <c r="N72">
         <v>0.4814285714285714</v>
       </c>
       <c r="O72">
-        <v>0.04357142857142857</v>
+        <v>0.04357142857142858</v>
       </c>
       <c r="P72">
         <v>0.205</v>
@@ -5662,16 +5662,16 @@
         <v>0.2175</v>
       </c>
       <c r="N73">
-        <v>0.46875</v>
+        <v>0.4687500000000001</v>
       </c>
       <c r="O73">
-        <v>0.04875000000000001</v>
+        <v>0.04875</v>
       </c>
       <c r="P73">
         <v>0.405</v>
       </c>
       <c r="Q73">
-        <v>0.720625</v>
+        <v>0.7206249999999998</v>
       </c>
       <c r="R73">
         <v>0.20625</v>
@@ -5730,7 +5730,7 @@
         <v>0.3383333333333333</v>
       </c>
       <c r="Q74">
-        <v>0.9466666666666667</v>
+        <v>0.9466666666666668</v>
       </c>
       <c r="R74">
         <v>0.1291666666666667</v>
@@ -5898,7 +5898,7 @@
         <v>0.2066666666666666</v>
       </c>
       <c r="N77">
-        <v>0.2441666666666666</v>
+        <v>0.2441666666666667</v>
       </c>
       <c r="O77">
         <v>0.04333333333333333</v>
@@ -5913,7 +5913,7 @@
         <v>0.3791666666666667</v>
       </c>
       <c r="S77">
-        <v>0.3116666666666667</v>
+        <v>0.3116666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>